<commit_message>
fixes to the historicla regulations
</commit_message>
<xml_diff>
--- a/data/sources/coho_regulations.xlsx
+++ b/data/sources/coho_regulations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\sport_harvest\sport\sport_harvest_estimator\data\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F9601C-1C5C-4147-B54B-285EE60D613E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F960066-A2E8-41E3-8CB8-A4E7D7F70CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="coho_regulations" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">coho_regulations!$A$1:$E$502</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">coho_regulations!$A$1:$E$492</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="8">
   <si>
     <t>regulation_type_code</t>
   </si>
@@ -471,11 +471,11 @@
   <sheetPr codeName="Sheet1" filterMode="1">
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:E502"/>
+  <dimension ref="A1:E492"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C198" sqref="C198"/>
+      <pane ySplit="1" topLeftCell="A245" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D359" sqref="D359"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,7 +521,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -538,7 +538,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -725,7 +725,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -844,7 +844,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -878,7 +878,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -929,7 +929,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -963,7 +963,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>7</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>7</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>5</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>7</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>7</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>7</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>7</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>5</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>7</v>
       </c>
@@ -2051,7 +2051,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>7</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>7</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="99" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>7</v>
       </c>
@@ -2170,7 +2170,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>5</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>7</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>7</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>7</v>
       </c>
@@ -2527,7 +2527,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="121" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>7</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>7</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>5</v>
       </c>
@@ -2782,7 +2782,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>7</v>
       </c>
@@ -2850,7 +2850,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>7</v>
       </c>
@@ -2952,7 +2952,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>7</v>
       </c>
@@ -2986,7 +2986,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="148" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>7</v>
       </c>
@@ -3054,7 +3054,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="152" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>7</v>
       </c>
@@ -3071,7 +3071,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>5</v>
       </c>
@@ -3241,7 +3241,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>7</v>
       </c>
@@ -3360,7 +3360,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="170" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>7</v>
       </c>
@@ -3394,7 +3394,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>7</v>
       </c>
@@ -3462,7 +3462,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="176" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>7</v>
       </c>
@@ -3479,7 +3479,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>5</v>
       </c>
@@ -3649,7 +3649,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>7</v>
       </c>
@@ -3700,7 +3700,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>7</v>
       </c>
@@ -3802,7 +3802,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="196" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>7</v>
       </c>
@@ -3836,7 +3836,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>7</v>
       </c>
@@ -3887,7 +3887,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="201" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>7</v>
       </c>
@@ -3904,7 +3904,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>5</v>
       </c>
@@ -4074,7 +4074,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>7</v>
       </c>
@@ -4108,7 +4108,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>7</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="218" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>7</v>
       </c>
@@ -4210,7 +4210,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>7</v>
       </c>
@@ -4261,7 +4261,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="223" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>7</v>
       </c>
@@ -4278,7 +4278,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>5</v>
       </c>
@@ -4448,7 +4448,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>7</v>
       </c>
@@ -4567,7 +4567,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="241" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>7</v>
       </c>
@@ -4601,7 +4601,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>7</v>
       </c>
@@ -4635,7 +4635,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="245" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>7</v>
       </c>
@@ -4652,7 +4652,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>5</v>
       </c>
@@ -4822,7 +4822,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>7</v>
       </c>
@@ -4924,7 +4924,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="262" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>7</v>
       </c>
@@ -4958,7 +4958,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>7</v>
       </c>
@@ -4992,7 +4992,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="266" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>7</v>
       </c>
@@ -5009,7 +5009,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>5</v>
       </c>
@@ -5179,7 +5179,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>7</v>
       </c>
@@ -5196,7 +5196,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>5</v>
       </c>
@@ -5275,7 +5275,7 @@
         <v>41974</v>
       </c>
       <c r="D282" s="6">
-        <v>42030</v>
+        <v>42124</v>
       </c>
       <c r="E282" t="s">
         <v>6</v>
@@ -5298,18 +5298,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="284" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>7</v>
       </c>
       <c r="B284">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C284" s="5">
-        <v>42034</v>
+        <v>42036</v>
       </c>
       <c r="D284" s="5">
-        <v>42036</v>
+        <v>42124</v>
       </c>
       <c r="E284" t="s">
         <v>6</v>
@@ -5320,7 +5320,7 @@
         <v>7</v>
       </c>
       <c r="B285">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C285" s="5">
         <v>42036</v>
@@ -5337,32 +5337,30 @@
         <v>7</v>
       </c>
       <c r="B286">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C286" s="5">
-        <v>42036</v>
+        <v>42051</v>
       </c>
       <c r="D286" s="5">
-        <v>42124</v>
+        <v>42104</v>
       </c>
       <c r="E286" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="287" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>7</v>
       </c>
       <c r="B287">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C287" s="5">
-        <f>C286+7</f>
-        <v>42043</v>
+        <v>42156</v>
       </c>
       <c r="D287" s="5">
-        <f>D286+7</f>
-        <v>42131</v>
+        <v>42369</v>
       </c>
       <c r="E287" t="s">
         <v>6</v>
@@ -5370,35 +5368,33 @@
     </row>
     <row r="288" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B288">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C288" s="5">
-        <f>C287+7</f>
-        <v>42050</v>
+        <v>42186</v>
       </c>
       <c r="D288" s="5">
-        <f>D287+7</f>
-        <v>42138</v>
+        <v>42258</v>
       </c>
       <c r="E288" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B289">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C289" s="5">
-        <v>42051</v>
+        <v>42186</v>
       </c>
       <c r="D289" s="5">
-        <v>42104</v>
+        <v>42277</v>
       </c>
       <c r="E289" t="s">
         <v>6</v>
@@ -5409,30 +5405,30 @@
         <v>7</v>
       </c>
       <c r="B290">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C290" s="5">
-        <v>42156</v>
+        <v>42186</v>
       </c>
       <c r="D290" s="5">
-        <v>42369</v>
+        <v>42338</v>
       </c>
       <c r="E290" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B291">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C291" s="5">
         <v>42186</v>
       </c>
       <c r="D291" s="5">
-        <v>42258</v>
+        <v>42292</v>
       </c>
       <c r="E291" t="s">
         <v>6</v>
@@ -5440,16 +5436,16 @@
     </row>
     <row r="292" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B292">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C292" s="5">
         <v>42186</v>
       </c>
       <c r="D292" s="5">
-        <v>42277</v>
+        <v>42369</v>
       </c>
       <c r="E292" t="s">
         <v>6</v>
@@ -5457,16 +5453,16 @@
     </row>
     <row r="293" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B293">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C293" s="5">
         <v>42186</v>
       </c>
       <c r="D293" s="5">
-        <v>42338</v>
+        <v>42277</v>
       </c>
       <c r="E293" t="s">
         <v>6</v>
@@ -5474,16 +5470,16 @@
     </row>
     <row r="294" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B294">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C294" s="5">
-        <v>42186</v>
+        <v>42217</v>
       </c>
       <c r="D294" s="5">
-        <v>42292</v>
+        <v>42277</v>
       </c>
       <c r="E294" t="s">
         <v>6</v>
@@ -5494,13 +5490,13 @@
         <v>7</v>
       </c>
       <c r="B295">
-        <v>12</v>
+        <v>81</v>
       </c>
       <c r="C295" s="5">
-        <v>42186</v>
+        <v>42217</v>
       </c>
       <c r="D295" s="5">
-        <v>42369</v>
+        <v>42338</v>
       </c>
       <c r="E295" t="s">
         <v>6</v>
@@ -5508,16 +5504,16 @@
     </row>
     <row r="296" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B296">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="C296" s="5">
-        <v>42186</v>
+        <v>42217</v>
       </c>
       <c r="D296" s="5">
-        <v>42277</v>
+        <v>42308</v>
       </c>
       <c r="E296" t="s">
         <v>6</v>
@@ -5525,33 +5521,30 @@
     </row>
     <row r="297" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B297">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C297" s="5">
-        <v>42217</v>
+        <v>42259</v>
       </c>
       <c r="D297" s="5">
-        <v>42277</v>
-      </c>
-      <c r="E297" t="s">
-        <v>6</v>
+        <v>42261</v>
       </c>
     </row>
     <row r="298" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B298">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="C298" s="5">
-        <v>42217</v>
+        <v>42262</v>
       </c>
       <c r="D298" s="5">
-        <v>42338</v>
+        <v>42265</v>
       </c>
       <c r="E298" t="s">
         <v>6</v>
@@ -5562,123 +5555,126 @@
         <v>7</v>
       </c>
       <c r="B299">
-        <v>82</v>
+        <v>5</v>
       </c>
       <c r="C299" s="5">
-        <v>42217</v>
+        <v>42266</v>
       </c>
       <c r="D299" s="5">
+        <v>42268</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
+        <v>5</v>
+      </c>
+      <c r="B300">
+        <v>5</v>
+      </c>
+      <c r="C300" s="5">
+        <v>42269</v>
+      </c>
+      <c r="D300" s="5">
+        <v>42272</v>
+      </c>
+      <c r="E300" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>7</v>
+      </c>
+      <c r="B301">
+        <v>5</v>
+      </c>
+      <c r="C301" s="5">
+        <v>42273</v>
+      </c>
+      <c r="D301" s="5">
+        <v>42274</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>5</v>
+      </c>
+      <c r="B302">
+        <v>5</v>
+      </c>
+      <c r="C302" s="5">
+        <v>42275</v>
+      </c>
+      <c r="D302" s="5">
+        <v>42277</v>
+      </c>
+      <c r="E302" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>7</v>
+      </c>
+      <c r="B303">
+        <v>6</v>
+      </c>
+      <c r="C303" s="5">
+        <v>42278</v>
+      </c>
+      <c r="D303" s="5">
         <v>42308</v>
       </c>
-      <c r="E299" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A300" t="s">
-        <v>7</v>
-      </c>
-      <c r="B300">
-        <v>5</v>
-      </c>
-      <c r="C300" s="5">
-        <v>42259</v>
-      </c>
-      <c r="D300" s="5">
-        <v>42261</v>
-      </c>
-    </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A301" t="s">
-        <v>5</v>
-      </c>
-      <c r="B301">
-        <v>5</v>
-      </c>
-      <c r="C301" s="5">
-        <v>42262</v>
-      </c>
-      <c r="D301" s="5">
-        <v>42265</v>
-      </c>
-      <c r="E301" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A302" t="s">
-        <v>7</v>
-      </c>
-      <c r="B302">
-        <v>5</v>
-      </c>
-      <c r="C302" s="5">
-        <v>42266</v>
-      </c>
-      <c r="D302" s="5">
-        <v>42268</v>
-      </c>
-    </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A303" t="s">
-        <v>5</v>
-      </c>
-      <c r="B303">
-        <v>5</v>
-      </c>
-      <c r="C303" s="5">
-        <v>42269</v>
-      </c>
-      <c r="D303" s="5">
-        <v>42272</v>
-      </c>
       <c r="E303" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>7</v>
       </c>
       <c r="B304">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C304" s="5">
-        <v>42273</v>
+        <v>42278</v>
       </c>
       <c r="D304" s="5">
-        <v>42274</v>
-      </c>
-    </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+        <v>42308</v>
+      </c>
+      <c r="E304" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>5</v>
       </c>
       <c r="B305">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C305" s="5">
-        <v>42275</v>
+        <v>42278</v>
       </c>
       <c r="D305" s="5">
-        <v>42277</v>
+        <v>42308</v>
       </c>
       <c r="E305" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="306" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>7</v>
       </c>
       <c r="B306">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C306" s="5">
-        <v>42278</v>
+        <v>42305</v>
       </c>
       <c r="D306" s="5">
-        <v>42308</v>
+        <v>42338</v>
       </c>
       <c r="E306" t="s">
         <v>6</v>
@@ -5689,13 +5685,13 @@
         <v>7</v>
       </c>
       <c r="B307">
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="C307" s="5">
-        <v>42278</v>
+        <v>42309</v>
       </c>
       <c r="D307" s="5">
-        <v>42308</v>
+        <v>42490</v>
       </c>
       <c r="E307" t="s">
         <v>6</v>
@@ -5703,16 +5699,16 @@
     </row>
     <row r="308" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B308">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C308" s="5">
-        <v>42278</v>
+        <v>42339</v>
       </c>
       <c r="D308" s="5">
-        <v>42308</v>
+        <v>42470</v>
       </c>
       <c r="E308" t="s">
         <v>6</v>
@@ -5723,13 +5719,13 @@
         <v>7</v>
       </c>
       <c r="B309">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C309" s="5">
-        <v>42305</v>
+        <v>42339</v>
       </c>
       <c r="D309" s="5">
-        <v>42338</v>
+        <v>42490</v>
       </c>
       <c r="E309" t="s">
         <v>6</v>
@@ -5740,13 +5736,13 @@
         <v>7</v>
       </c>
       <c r="B310">
-        <v>82</v>
+        <v>10</v>
       </c>
       <c r="C310" s="5">
-        <v>42309</v>
+        <v>42339</v>
       </c>
       <c r="D310" s="5">
-        <v>42490</v>
+        <v>42400</v>
       </c>
       <c r="E310" t="s">
         <v>6</v>
@@ -5757,13 +5753,13 @@
         <v>7</v>
       </c>
       <c r="B311">
-        <v>6</v>
+        <v>81</v>
       </c>
       <c r="C311" s="5">
         <v>42339</v>
       </c>
       <c r="D311" s="5">
-        <v>42470</v>
+        <v>42490</v>
       </c>
       <c r="E311" t="s">
         <v>6</v>
@@ -5774,30 +5770,30 @@
         <v>7</v>
       </c>
       <c r="B312">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C312" s="5">
-        <v>42339</v>
+        <v>42385</v>
       </c>
       <c r="D312" s="5">
+        <v>42475</v>
+      </c>
+      <c r="E312" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
+        <v>7</v>
+      </c>
+      <c r="B313">
+        <v>11</v>
+      </c>
+      <c r="C313" s="5">
+        <v>42401</v>
+      </c>
+      <c r="D313" s="5">
         <v>42490</v>
-      </c>
-      <c r="E312" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="313" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A313" t="s">
-        <v>7</v>
-      </c>
-      <c r="B313">
-        <v>10</v>
-      </c>
-      <c r="C313" s="5">
-        <v>42339</v>
-      </c>
-      <c r="D313" s="5">
-        <v>42400</v>
       </c>
       <c r="E313" t="s">
         <v>6</v>
@@ -5808,10 +5804,10 @@
         <v>7</v>
       </c>
       <c r="B314">
-        <v>81</v>
+        <v>12</v>
       </c>
       <c r="C314" s="5">
-        <v>42339</v>
+        <v>42401</v>
       </c>
       <c r="D314" s="5">
         <v>42490</v>
@@ -5825,13 +5821,13 @@
         <v>7</v>
       </c>
       <c r="B315">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C315" s="5">
-        <v>42385</v>
+        <v>42416</v>
       </c>
       <c r="D315" s="5">
-        <v>42475</v>
+        <v>42490</v>
       </c>
       <c r="E315" t="s">
         <v>6</v>
@@ -5842,13 +5838,13 @@
         <v>7</v>
       </c>
       <c r="B316">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C316" s="5">
-        <v>42401</v>
+        <v>42552</v>
       </c>
       <c r="D316" s="5">
-        <v>42490</v>
+        <v>42674</v>
       </c>
       <c r="E316" t="s">
         <v>6</v>
@@ -5856,33 +5852,33 @@
     </row>
     <row r="317" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B317">
+        <v>13</v>
+      </c>
+      <c r="C317" s="5">
+        <v>42644</v>
+      </c>
+      <c r="D317" s="5">
+        <v>42664</v>
+      </c>
+      <c r="E317" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="318" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A318" t="s">
+        <v>7</v>
+      </c>
+      <c r="B318">
         <v>12</v>
       </c>
-      <c r="C317" s="5">
-        <v>42401</v>
-      </c>
-      <c r="D317" s="5">
-        <v>42490</v>
-      </c>
-      <c r="E317" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A318" t="s">
-        <v>7</v>
-      </c>
-      <c r="B318">
-        <v>5</v>
-      </c>
       <c r="C318" s="5">
-        <v>42416</v>
+        <v>42675</v>
       </c>
       <c r="D318" s="5">
-        <v>42490</v>
+        <v>42855</v>
       </c>
       <c r="E318" t="s">
         <v>6</v>
@@ -5890,33 +5886,33 @@
     </row>
     <row r="319" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B319">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C319" s="5">
-        <v>42552</v>
+        <v>42856</v>
       </c>
       <c r="D319" s="5">
-        <v>42674</v>
+        <v>43008</v>
       </c>
       <c r="E319" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="320" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B320">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C320" s="5">
-        <v>42644</v>
+        <v>42887</v>
       </c>
       <c r="D320" s="5">
-        <v>42664</v>
+        <v>43039</v>
       </c>
       <c r="E320" t="s">
         <v>6</v>
@@ -5924,16 +5920,16 @@
     </row>
     <row r="321" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B321">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C321" s="5">
-        <v>42675</v>
+        <v>42917</v>
       </c>
       <c r="D321" s="5">
-        <v>42855</v>
+        <v>42978</v>
       </c>
       <c r="E321" t="s">
         <v>6</v>
@@ -5944,13 +5940,13 @@
         <v>5</v>
       </c>
       <c r="B322">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C322" s="5">
-        <v>42856</v>
+        <v>42917</v>
       </c>
       <c r="D322" s="5">
-        <v>43008</v>
+        <v>42962</v>
       </c>
       <c r="E322" t="s">
         <v>6</v>
@@ -5961,30 +5957,30 @@
         <v>7</v>
       </c>
       <c r="B323">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C323" s="5">
-        <v>42887</v>
+        <v>42917</v>
       </c>
       <c r="D323" s="5">
-        <v>43039</v>
+        <v>43008</v>
       </c>
       <c r="E323" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B324">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C324" s="5">
         <v>42917</v>
       </c>
       <c r="D324" s="5">
-        <v>42978</v>
+        <v>43069</v>
       </c>
       <c r="E324" t="s">
         <v>6</v>
@@ -5995,13 +5991,13 @@
         <v>5</v>
       </c>
       <c r="B325">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C325" s="5">
-        <v>42917</v>
+        <v>42932</v>
       </c>
       <c r="D325" s="5">
-        <v>42962</v>
+        <v>42982</v>
       </c>
       <c r="E325" t="s">
         <v>6</v>
@@ -6009,16 +6005,16 @@
     </row>
     <row r="326" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B326">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C326" s="5">
         <v>42917</v>
       </c>
       <c r="D326" s="5">
-        <v>43008</v>
+        <v>43159</v>
       </c>
       <c r="E326" t="s">
         <v>6</v>
@@ -6026,16 +6022,16 @@
     </row>
     <row r="327" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B327">
-        <v>12</v>
+        <v>82</v>
       </c>
       <c r="C327" s="5">
-        <v>42917</v>
+        <v>42948</v>
       </c>
       <c r="D327" s="5">
-        <v>43069</v>
+        <v>42982</v>
       </c>
       <c r="E327" t="s">
         <v>6</v>
@@ -6046,30 +6042,30 @@
         <v>5</v>
       </c>
       <c r="B328">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C328" s="5">
-        <v>42932</v>
+        <v>43009</v>
       </c>
       <c r="D328" s="5">
-        <v>42982</v>
+        <v>43220</v>
       </c>
       <c r="E328" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="329" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>5</v>
       </c>
       <c r="B329">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C329" s="5">
-        <v>42932</v>
+        <v>43040</v>
       </c>
       <c r="D329" s="5">
-        <v>43039</v>
+        <v>43220</v>
       </c>
       <c r="E329" t="s">
         <v>6</v>
@@ -6077,16 +6073,16 @@
     </row>
     <row r="330" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B330">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="C330" s="5">
-        <v>42948</v>
+        <v>43070</v>
       </c>
       <c r="D330" s="5">
-        <v>42982</v>
+        <v>43220</v>
       </c>
       <c r="E330" t="s">
         <v>6</v>
@@ -6100,27 +6096,27 @@
         <v>13</v>
       </c>
       <c r="C331" s="5">
-        <v>43009</v>
+        <v>43221</v>
       </c>
       <c r="D331" s="5">
-        <v>43220</v>
+        <v>43373</v>
       </c>
       <c r="E331" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="332" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B332">
         <v>11</v>
       </c>
       <c r="C332" s="5">
-        <v>43040</v>
+        <v>43252</v>
       </c>
       <c r="D332" s="5">
-        <v>43220</v>
+        <v>43297</v>
       </c>
       <c r="E332" t="s">
         <v>6</v>
@@ -6128,16 +6124,16 @@
     </row>
     <row r="333" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B333">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C333" s="5">
-        <v>43070</v>
+        <v>43282</v>
       </c>
       <c r="D333" s="5">
-        <v>43220</v>
+        <v>43373</v>
       </c>
       <c r="E333" t="s">
         <v>6</v>
@@ -6148,10 +6144,10 @@
         <v>5</v>
       </c>
       <c r="B334">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C334" s="5">
-        <v>43221</v>
+        <v>43282</v>
       </c>
       <c r="D334" s="5">
         <v>43373</v>
@@ -6165,30 +6161,30 @@
         <v>7</v>
       </c>
       <c r="B335">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C335" s="5">
-        <v>43252</v>
+        <v>43282</v>
       </c>
       <c r="D335" s="5">
-        <v>43297</v>
+        <v>43373</v>
       </c>
       <c r="E335" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B336">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C336" s="5">
         <v>43282</v>
       </c>
       <c r="D336" s="5">
-        <v>43373</v>
+        <v>43419</v>
       </c>
       <c r="E336" t="s">
         <v>6</v>
@@ -6196,16 +6192,16 @@
     </row>
     <row r="337" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B337">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C337" s="5">
         <v>43282</v>
       </c>
       <c r="D337" s="5">
-        <v>43373</v>
+        <v>43404</v>
       </c>
       <c r="E337" t="s">
         <v>6</v>
@@ -6213,13 +6209,13 @@
     </row>
     <row r="338" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B338">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C338" s="5">
-        <v>43282</v>
+        <v>43297</v>
       </c>
       <c r="D338" s="5">
         <v>43373</v>
@@ -6228,49 +6224,49 @@
         <v>6</v>
       </c>
     </row>
-    <row r="339" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>7</v>
       </c>
       <c r="B339">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C339" s="5">
-        <v>43282</v>
+        <v>43301</v>
       </c>
       <c r="D339" s="5">
-        <v>43419</v>
+        <v>43304</v>
       </c>
       <c r="E339" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="340" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>7</v>
       </c>
       <c r="B340">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C340" s="5">
-        <v>43282</v>
+        <v>43308</v>
       </c>
       <c r="D340" s="5">
-        <v>43769</v>
+        <v>43311</v>
       </c>
       <c r="E340" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="341" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B341">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C341" s="5">
-        <v>43297</v>
+        <v>43312</v>
       </c>
       <c r="D341" s="5">
         <v>43373</v>
@@ -6284,13 +6280,13 @@
         <v>7</v>
       </c>
       <c r="B342">
-        <v>11</v>
+        <v>81</v>
       </c>
       <c r="C342" s="5">
-        <v>43301</v>
+        <v>43313</v>
       </c>
       <c r="D342" s="5">
-        <v>43304</v>
+        <v>43373</v>
       </c>
       <c r="E342" t="s">
         <v>6</v>
@@ -6301,13 +6297,13 @@
         <v>7</v>
       </c>
       <c r="B343">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="C343" s="5">
-        <v>43308</v>
+        <v>43313</v>
       </c>
       <c r="D343" s="5">
-        <v>43311</v>
+        <v>43366</v>
       </c>
       <c r="E343" t="s">
         <v>6</v>
@@ -6315,16 +6311,16 @@
     </row>
     <row r="344" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B344">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C344" s="5">
-        <v>43312</v>
+        <v>43374</v>
       </c>
       <c r="D344" s="5">
-        <v>43373</v>
+        <v>43585</v>
       </c>
       <c r="E344" t="s">
         <v>6</v>
@@ -6335,30 +6331,30 @@
         <v>7</v>
       </c>
       <c r="B345">
-        <v>81</v>
+        <v>12</v>
       </c>
       <c r="C345" s="5">
-        <v>43313</v>
+        <v>43405</v>
       </c>
       <c r="D345" s="5">
-        <v>43373</v>
+        <v>43585</v>
       </c>
       <c r="E345" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="346" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>7</v>
       </c>
       <c r="B346">
-        <v>82</v>
+        <v>11</v>
       </c>
       <c r="C346" s="5">
-        <v>43313</v>
+        <v>43374</v>
       </c>
       <c r="D346" s="5">
-        <v>43366</v>
+        <v>43585</v>
       </c>
       <c r="E346" t="s">
         <v>6</v>
@@ -6366,16 +6362,16 @@
     </row>
     <row r="347" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B347">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C347" s="5">
-        <v>43374</v>
+        <v>43466</v>
       </c>
       <c r="D347" s="5">
-        <v>43585</v>
+        <v>43555</v>
       </c>
       <c r="E347" t="s">
         <v>6</v>
@@ -6383,16 +6379,16 @@
     </row>
     <row r="348" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B348">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C348" s="5">
-        <v>43405</v>
+        <v>43497</v>
       </c>
       <c r="D348" s="5">
-        <v>43585</v>
+        <v>43570</v>
       </c>
       <c r="E348" t="s">
         <v>6</v>
@@ -6400,13 +6396,13 @@
     </row>
     <row r="349" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B349">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C349" s="5">
-        <v>43435</v>
+        <v>43512</v>
       </c>
       <c r="D349" s="5">
         <v>43585</v>
@@ -6417,16 +6413,16 @@
     </row>
     <row r="350" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B350">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C350" s="5">
-        <v>43466</v>
+        <v>43586</v>
       </c>
       <c r="D350" s="5">
-        <v>43555</v>
+        <v>43738</v>
       </c>
       <c r="E350" t="s">
         <v>6</v>
@@ -6434,22 +6430,22 @@
     </row>
     <row r="351" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B351">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C351" s="5">
-        <v>43497</v>
+        <v>43617</v>
       </c>
       <c r="D351" s="5">
-        <v>43570</v>
+        <v>43784</v>
       </c>
       <c r="E351" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>5</v>
       </c>
@@ -6457,10 +6453,10 @@
         <v>5</v>
       </c>
       <c r="C352" s="5">
-        <v>43512</v>
+        <v>43647</v>
       </c>
       <c r="D352" s="5">
-        <v>43585</v>
+        <v>43738</v>
       </c>
       <c r="E352" t="s">
         <v>6</v>
@@ -6471,10 +6467,10 @@
         <v>5</v>
       </c>
       <c r="B353">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C353" s="5">
-        <v>43586</v>
+        <v>43647</v>
       </c>
       <c r="D353" s="5">
         <v>43738</v>
@@ -6488,13 +6484,13 @@
         <v>7</v>
       </c>
       <c r="B354">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C354" s="5">
-        <v>43617</v>
+        <v>43647</v>
       </c>
       <c r="D354" s="5">
-        <v>43784</v>
+        <v>43677</v>
       </c>
       <c r="E354" t="s">
         <v>6</v>
@@ -6502,16 +6498,16 @@
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B355">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C355" s="5">
         <v>43647</v>
       </c>
       <c r="D355" s="5">
-        <v>43738</v>
+        <v>43649</v>
       </c>
       <c r="E355" t="s">
         <v>6</v>
@@ -6519,39 +6515,39 @@
     </row>
     <row r="356" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B356">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C356" s="5">
         <v>43647</v>
       </c>
       <c r="D356" s="5">
-        <v>43738</v>
+        <v>43769</v>
       </c>
       <c r="E356" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="357" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>7</v>
       </c>
       <c r="B357">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C357" s="5">
-        <v>43647</v>
+        <v>43652</v>
       </c>
       <c r="D357" s="5">
-        <v>43677</v>
+        <v>43656</v>
       </c>
       <c r="E357" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="358" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>7</v>
       </c>
@@ -6559,27 +6555,27 @@
         <v>11</v>
       </c>
       <c r="C358" s="5">
-        <v>43647</v>
+        <v>43659</v>
       </c>
       <c r="D358" s="5">
-        <v>43649</v>
+        <v>43663</v>
       </c>
       <c r="E358" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="359" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>7</v>
       </c>
       <c r="B359">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C359" s="5">
-        <v>43647</v>
+        <v>43666</v>
       </c>
       <c r="D359" s="5">
-        <v>43769</v>
+        <v>43670</v>
       </c>
       <c r="E359" t="s">
         <v>6</v>
@@ -6587,22 +6583,22 @@
     </row>
     <row r="360" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B360">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C360" s="5">
-        <v>43652</v>
+        <v>43671</v>
       </c>
       <c r="D360" s="5">
-        <v>43656</v>
+        <v>43738</v>
       </c>
       <c r="E360" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="361" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>7</v>
       </c>
@@ -6610,10 +6606,10 @@
         <v>11</v>
       </c>
       <c r="C361" s="5">
-        <v>43659</v>
+        <v>43673</v>
       </c>
       <c r="D361" s="5">
-        <v>43663</v>
+        <v>43677</v>
       </c>
       <c r="E361" t="s">
         <v>6</v>
@@ -6624,36 +6620,36 @@
         <v>7</v>
       </c>
       <c r="B362">
+        <v>81</v>
+      </c>
+      <c r="C362" s="5">
+        <v>43678</v>
+      </c>
+      <c r="D362" s="5">
+        <v>43769</v>
+      </c>
+      <c r="E362" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A363" t="s">
+        <v>7</v>
+      </c>
+      <c r="B363">
         <v>11</v>
       </c>
-      <c r="C362" s="5">
-        <v>43666</v>
-      </c>
-      <c r="D362" s="5">
-        <v>43670</v>
-      </c>
-      <c r="E362" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="363" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A363" t="s">
-        <v>5</v>
-      </c>
-      <c r="B363">
-        <v>9</v>
-      </c>
       <c r="C363" s="5">
-        <v>43671</v>
+        <v>43680</v>
       </c>
       <c r="D363" s="5">
-        <v>43738</v>
+        <v>43684</v>
       </c>
       <c r="E363" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="364" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>7</v>
       </c>
@@ -6661,10 +6657,10 @@
         <v>11</v>
       </c>
       <c r="C364" s="5">
-        <v>43673</v>
+        <v>43687</v>
       </c>
       <c r="D364" s="5">
-        <v>43677</v>
+        <v>43691</v>
       </c>
       <c r="E364" t="s">
         <v>6</v>
@@ -6672,22 +6668,22 @@
     </row>
     <row r="365" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B365">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C365" s="5">
-        <v>43678</v>
+        <v>43693</v>
       </c>
       <c r="D365" s="5">
-        <v>43769</v>
+        <v>43723</v>
       </c>
       <c r="E365" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="366" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>7</v>
       </c>
@@ -6695,16 +6691,16 @@
         <v>11</v>
       </c>
       <c r="C366" s="5">
-        <v>43680</v>
+        <v>43694</v>
       </c>
       <c r="D366" s="5">
-        <v>43684</v>
+        <v>43698</v>
       </c>
       <c r="E366" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="367" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>7</v>
       </c>
@@ -6712,27 +6708,27 @@
         <v>11</v>
       </c>
       <c r="C367" s="5">
-        <v>43687</v>
+        <v>43701</v>
       </c>
       <c r="D367" s="5">
-        <v>43691</v>
+        <v>43702</v>
       </c>
       <c r="E367" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="368" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B368">
-        <v>82</v>
+        <v>11</v>
       </c>
       <c r="C368" s="5">
-        <v>43693</v>
+        <v>43703</v>
       </c>
       <c r="D368" s="5">
-        <v>43723</v>
+        <v>43738</v>
       </c>
       <c r="E368" t="s">
         <v>6</v>
@@ -6743,13 +6739,13 @@
         <v>7</v>
       </c>
       <c r="B369">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C369" s="5">
-        <v>43694</v>
+        <v>43709</v>
       </c>
       <c r="D369" s="5">
-        <v>43698</v>
+        <v>43738</v>
       </c>
       <c r="E369" t="s">
         <v>6</v>
@@ -6757,16 +6753,16 @@
     </row>
     <row r="370" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B370">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C370" s="5">
-        <v>43701</v>
+        <v>43739</v>
       </c>
       <c r="D370" s="5">
-        <v>43702</v>
+        <v>43914</v>
       </c>
       <c r="E370" t="s">
         <v>6</v>
@@ -6777,13 +6773,13 @@
         <v>7</v>
       </c>
       <c r="B371">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C371" s="5">
-        <v>43703</v>
+        <v>43770</v>
       </c>
       <c r="D371" s="5">
-        <v>43738</v>
+        <v>43951</v>
       </c>
       <c r="E371" t="s">
         <v>6</v>
@@ -6794,30 +6790,30 @@
         <v>7</v>
       </c>
       <c r="B372">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C372" s="5">
-        <v>43709</v>
+        <v>43831</v>
       </c>
       <c r="D372" s="5">
-        <v>43738</v>
+        <v>43914</v>
       </c>
       <c r="E372" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="373" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B373">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C373" s="5">
-        <v>43739</v>
+        <v>43831</v>
       </c>
       <c r="D373" s="5">
-        <v>43914</v>
+        <v>43951</v>
       </c>
       <c r="E373" t="s">
         <v>6</v>
@@ -6825,16 +6821,16 @@
     </row>
     <row r="374" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B374">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C374" s="5">
-        <v>43770</v>
+        <v>43862</v>
       </c>
       <c r="D374" s="5">
-        <v>43951</v>
+        <v>43914</v>
       </c>
       <c r="E374" t="s">
         <v>6</v>
@@ -6842,13 +6838,13 @@
     </row>
     <row r="375" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B375">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C375" s="5">
-        <v>43831</v>
+        <v>43891</v>
       </c>
       <c r="D375" s="5">
         <v>43914</v>
@@ -6859,16 +6855,16 @@
     </row>
     <row r="376" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B376">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C376" s="5">
-        <v>43831</v>
+        <v>43891</v>
       </c>
       <c r="D376" s="5">
-        <v>43951</v>
+        <v>43914</v>
       </c>
       <c r="E376" t="s">
         <v>6</v>
@@ -6879,30 +6875,30 @@
         <v>5</v>
       </c>
       <c r="B377">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C377" s="5">
-        <v>43862</v>
+        <v>43958</v>
       </c>
       <c r="D377" s="5">
-        <v>43914</v>
+        <v>44104</v>
       </c>
       <c r="E377" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B378">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C378" s="5">
-        <v>43891</v>
+        <v>43983</v>
       </c>
       <c r="D378" s="5">
-        <v>43914</v>
+        <v>44150</v>
       </c>
       <c r="E378" t="s">
         <v>6</v>
@@ -6913,13 +6909,13 @@
         <v>5</v>
       </c>
       <c r="B379">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C379" s="5">
-        <v>43891</v>
+        <v>44013</v>
       </c>
       <c r="D379" s="5">
-        <v>43914</v>
+        <v>44104</v>
       </c>
       <c r="E379" t="s">
         <v>6</v>
@@ -6930,10 +6926,10 @@
         <v>5</v>
       </c>
       <c r="B380">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C380" s="5">
-        <v>43958</v>
+        <v>44013</v>
       </c>
       <c r="D380" s="5">
         <v>44104</v>
@@ -6947,13 +6943,13 @@
         <v>7</v>
       </c>
       <c r="B381">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C381" s="5">
-        <v>43983</v>
+        <v>44013</v>
       </c>
       <c r="D381" s="5">
-        <v>44150</v>
+        <v>44104</v>
       </c>
       <c r="E381" t="s">
         <v>6</v>
@@ -6961,16 +6957,16 @@
     </row>
     <row r="382" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B382">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C382" s="5">
         <v>44013</v>
       </c>
       <c r="D382" s="5">
-        <v>44104</v>
+        <v>44135</v>
       </c>
       <c r="E382" t="s">
         <v>6</v>
@@ -6978,16 +6974,16 @@
     </row>
     <row r="383" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B383">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C383" s="5">
         <v>44013</v>
       </c>
       <c r="D383" s="5">
-        <v>44104</v>
+        <v>44135</v>
       </c>
       <c r="E383" t="s">
         <v>6</v>
@@ -6995,13 +6991,13 @@
     </row>
     <row r="384" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B384">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C384" s="5">
-        <v>44013</v>
+        <v>44028</v>
       </c>
       <c r="D384" s="5">
         <v>44104</v>
@@ -7012,16 +7008,16 @@
     </row>
     <row r="385" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B385">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C385" s="5">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="D385" s="5">
-        <v>44135</v>
+        <v>44316</v>
       </c>
       <c r="E385" t="s">
         <v>6</v>
@@ -7032,13 +7028,13 @@
         <v>7</v>
       </c>
       <c r="B386">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C386" s="5">
-        <v>44013</v>
+        <v>44197</v>
       </c>
       <c r="D386" s="5">
-        <v>44135</v>
+        <v>44214</v>
       </c>
       <c r="E386" t="s">
         <v>6</v>
@@ -7049,13 +7045,13 @@
         <v>5</v>
       </c>
       <c r="B387">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C387" s="5">
-        <v>44028</v>
+        <v>44256</v>
       </c>
       <c r="D387" s="5">
-        <v>44104</v>
+        <v>44316</v>
       </c>
       <c r="E387" t="s">
         <v>6</v>
@@ -7069,10 +7065,10 @@
         <v>13</v>
       </c>
       <c r="C388" s="5">
-        <v>44105</v>
+        <v>44317</v>
       </c>
       <c r="D388" s="5">
-        <v>44316</v>
+        <v>44469</v>
       </c>
       <c r="E388" t="s">
         <v>6</v>
@@ -7086,10 +7082,10 @@
         <v>10</v>
       </c>
       <c r="C389" s="5">
-        <v>44197</v>
+        <v>44363</v>
       </c>
       <c r="D389" s="5">
-        <v>44214</v>
+        <v>44500</v>
       </c>
       <c r="E389" t="s">
         <v>6</v>
@@ -7097,16 +7093,16 @@
     </row>
     <row r="390" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B390">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C390" s="5">
-        <v>44256</v>
+        <v>44363</v>
       </c>
       <c r="D390" s="5">
-        <v>44316</v>
+        <v>44469</v>
       </c>
       <c r="E390" t="s">
         <v>6</v>
@@ -7117,10 +7113,10 @@
         <v>5</v>
       </c>
       <c r="B391">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C391" s="5">
-        <v>44317</v>
+        <v>44378</v>
       </c>
       <c r="D391" s="5">
         <v>44469</v>
@@ -7131,16 +7127,16 @@
     </row>
     <row r="392" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B392">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C392" s="5">
-        <v>44363</v>
+        <v>44378</v>
       </c>
       <c r="D392" s="5">
-        <v>44500</v>
+        <v>44469</v>
       </c>
       <c r="E392" t="s">
         <v>6</v>
@@ -7148,27 +7144,27 @@
     </row>
     <row r="393" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B393">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C393" s="5">
-        <v>44363</v>
+        <v>44378</v>
       </c>
       <c r="D393" s="5">
-        <v>44469</v>
+        <v>44384</v>
       </c>
       <c r="E393" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="394" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B394">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C394" s="5">
         <v>44378</v>
@@ -7185,10 +7181,10 @@
         <v>5</v>
       </c>
       <c r="B395">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C395" s="5">
-        <v>44378</v>
+        <v>44393</v>
       </c>
       <c r="D395" s="5">
         <v>44469</v>
@@ -7199,16 +7195,16 @@
     </row>
     <row r="396" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B396">
-        <v>7</v>
+        <v>81</v>
       </c>
       <c r="C396" s="5">
-        <v>44378</v>
+        <v>44409</v>
       </c>
       <c r="D396" s="5">
-        <v>44384</v>
+        <v>44458</v>
       </c>
       <c r="E396" t="s">
         <v>6</v>
@@ -7216,36 +7212,33 @@
     </row>
     <row r="397" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B397">
-        <v>12</v>
+        <v>82</v>
       </c>
       <c r="C397" s="5">
-        <v>44378</v>
+        <v>44422</v>
       </c>
       <c r="D397" s="5">
-        <v>44469</v>
+        <v>44458</v>
       </c>
       <c r="E397" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="398" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B398">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C398" s="5">
-        <v>44393</v>
+        <v>44470</v>
       </c>
       <c r="D398" s="5">
-        <v>44469</v>
-      </c>
-      <c r="E398" t="s">
-        <v>6</v>
+        <v>44500</v>
       </c>
     </row>
     <row r="399" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -7253,16 +7246,13 @@
         <v>7</v>
       </c>
       <c r="B399">
-        <v>81</v>
+        <v>12</v>
       </c>
       <c r="C399" s="5">
-        <v>44409</v>
+        <v>44470</v>
       </c>
       <c r="D399" s="5">
-        <v>44458</v>
-      </c>
-      <c r="E399" t="s">
-        <v>6</v>
+        <v>44530</v>
       </c>
     </row>
     <row r="400" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -7270,13 +7260,13 @@
         <v>5</v>
       </c>
       <c r="B400">
-        <v>82</v>
+        <v>13</v>
       </c>
       <c r="C400" s="5">
-        <v>44422</v>
+        <v>44470</v>
       </c>
       <c r="D400" s="5">
-        <v>44458</v>
+        <v>44681</v>
       </c>
       <c r="E400" t="s">
         <v>6</v>
@@ -7290,10 +7280,10 @@
         <v>10</v>
       </c>
       <c r="C401" s="5">
-        <v>44470</v>
+        <v>44562</v>
       </c>
       <c r="D401" s="5">
-        <v>44500</v>
+        <v>44563</v>
       </c>
       <c r="E401" t="s">
         <v>6</v>
@@ -7304,13 +7294,16 @@
         <v>7</v>
       </c>
       <c r="B402">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C402" s="5">
-        <v>44470</v>
+        <v>44564</v>
       </c>
       <c r="D402" s="5">
-        <v>44500</v>
+        <v>44564</v>
+      </c>
+      <c r="E402" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="403" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -7318,27 +7311,30 @@
         <v>7</v>
       </c>
       <c r="B403">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C403" s="5">
-        <v>44470</v>
+        <v>44569</v>
       </c>
       <c r="D403" s="5">
-        <v>44530</v>
+        <v>44569</v>
+      </c>
+      <c r="E403" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="404" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B404">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C404" s="5">
-        <v>44470</v>
+        <v>44570</v>
       </c>
       <c r="D404" s="5">
-        <v>44681</v>
+        <v>44570</v>
       </c>
       <c r="E404" t="s">
         <v>6</v>
@@ -7352,10 +7348,10 @@
         <v>10</v>
       </c>
       <c r="C405" s="5">
-        <v>44562</v>
+        <v>44571</v>
       </c>
       <c r="D405" s="5">
-        <v>44563</v>
+        <v>44571</v>
       </c>
       <c r="E405" t="s">
         <v>6</v>
@@ -7369,10 +7365,10 @@
         <v>10</v>
       </c>
       <c r="C406" s="5">
-        <v>44564</v>
+        <v>44616</v>
       </c>
       <c r="D406" s="5">
-        <v>44564</v>
+        <v>44616</v>
       </c>
       <c r="E406" t="s">
         <v>6</v>
@@ -7386,10 +7382,10 @@
         <v>10</v>
       </c>
       <c r="C407" s="5">
-        <v>44569</v>
+        <v>44617</v>
       </c>
       <c r="D407" s="5">
-        <v>44569</v>
+        <v>44617</v>
       </c>
       <c r="E407" t="s">
         <v>6</v>
@@ -7403,10 +7399,10 @@
         <v>10</v>
       </c>
       <c r="C408" s="5">
-        <v>44570</v>
+        <v>44618</v>
       </c>
       <c r="D408" s="5">
-        <v>44570</v>
+        <v>44618</v>
       </c>
       <c r="E408" t="s">
         <v>6</v>
@@ -7420,10 +7416,10 @@
         <v>10</v>
       </c>
       <c r="C409" s="5">
-        <v>44571</v>
+        <v>44623</v>
       </c>
       <c r="D409" s="5">
-        <v>44571</v>
+        <v>44623</v>
       </c>
       <c r="E409" t="s">
         <v>6</v>
@@ -7437,10 +7433,10 @@
         <v>10</v>
       </c>
       <c r="C410" s="5">
-        <v>44616</v>
+        <v>44624</v>
       </c>
       <c r="D410" s="5">
-        <v>44616</v>
+        <v>44624</v>
       </c>
       <c r="E410" t="s">
         <v>6</v>
@@ -7454,10 +7450,10 @@
         <v>10</v>
       </c>
       <c r="C411" s="5">
-        <v>44617</v>
+        <v>44625</v>
       </c>
       <c r="D411" s="5">
-        <v>44617</v>
+        <v>44625</v>
       </c>
       <c r="E411" t="s">
         <v>6</v>
@@ -7471,10 +7467,10 @@
         <v>10</v>
       </c>
       <c r="C412" s="5">
-        <v>44618</v>
+        <v>44630</v>
       </c>
       <c r="D412" s="5">
-        <v>44618</v>
+        <v>44630</v>
       </c>
       <c r="E412" t="s">
         <v>6</v>
@@ -7488,10 +7484,10 @@
         <v>10</v>
       </c>
       <c r="C413" s="5">
-        <v>44623</v>
+        <v>44631</v>
       </c>
       <c r="D413" s="5">
-        <v>44623</v>
+        <v>44631</v>
       </c>
       <c r="E413" t="s">
         <v>6</v>
@@ -7505,10 +7501,10 @@
         <v>10</v>
       </c>
       <c r="C414" s="5">
-        <v>44624</v>
+        <v>44632</v>
       </c>
       <c r="D414" s="5">
-        <v>44624</v>
+        <v>44632</v>
       </c>
       <c r="E414" t="s">
         <v>6</v>
@@ -7522,10 +7518,10 @@
         <v>10</v>
       </c>
       <c r="C415" s="5">
-        <v>44625</v>
+        <v>44636</v>
       </c>
       <c r="D415" s="5">
-        <v>44625</v>
+        <v>44637</v>
       </c>
       <c r="E415" t="s">
         <v>6</v>
@@ -7539,10 +7535,10 @@
         <v>10</v>
       </c>
       <c r="C416" s="5">
-        <v>44630</v>
+        <v>44638</v>
       </c>
       <c r="D416" s="5">
-        <v>44630</v>
+        <v>44638</v>
       </c>
       <c r="E416" t="s">
         <v>6</v>
@@ -7556,10 +7552,10 @@
         <v>10</v>
       </c>
       <c r="C417" s="5">
-        <v>44631</v>
+        <v>44639</v>
       </c>
       <c r="D417" s="5">
-        <v>44631</v>
+        <v>44639</v>
       </c>
       <c r="E417" t="s">
         <v>6</v>
@@ -7573,10 +7569,10 @@
         <v>10</v>
       </c>
       <c r="C418" s="5">
-        <v>44632</v>
+        <v>44640</v>
       </c>
       <c r="D418" s="5">
-        <v>44632</v>
+        <v>44640</v>
       </c>
       <c r="E418" t="s">
         <v>6</v>
@@ -7590,10 +7586,10 @@
         <v>10</v>
       </c>
       <c r="C419" s="5">
-        <v>44636</v>
+        <v>44641</v>
       </c>
       <c r="D419" s="5">
-        <v>44637</v>
+        <v>44644</v>
       </c>
       <c r="E419" t="s">
         <v>6</v>
@@ -7607,10 +7603,10 @@
         <v>10</v>
       </c>
       <c r="C420" s="5">
-        <v>44638</v>
+        <v>44645</v>
       </c>
       <c r="D420" s="5">
-        <v>44638</v>
+        <v>44645</v>
       </c>
       <c r="E420" t="s">
         <v>6</v>
@@ -7624,10 +7620,10 @@
         <v>10</v>
       </c>
       <c r="C421" s="5">
-        <v>44639</v>
+        <v>44646</v>
       </c>
       <c r="D421" s="5">
-        <v>44639</v>
+        <v>44646</v>
       </c>
       <c r="E421" t="s">
         <v>6</v>
@@ -7641,10 +7637,10 @@
         <v>10</v>
       </c>
       <c r="C422" s="5">
-        <v>44640</v>
+        <v>44647</v>
       </c>
       <c r="D422" s="5">
-        <v>44640</v>
+        <v>44647</v>
       </c>
       <c r="E422" t="s">
         <v>6</v>
@@ -7658,10 +7654,10 @@
         <v>10</v>
       </c>
       <c r="C423" s="5">
-        <v>44641</v>
+        <v>44648</v>
       </c>
       <c r="D423" s="5">
-        <v>44644</v>
+        <v>44651</v>
       </c>
       <c r="E423" t="s">
         <v>6</v>
@@ -7669,53 +7665,47 @@
     </row>
     <row r="424" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B424">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C424" s="5">
-        <v>44645</v>
+        <v>44700</v>
       </c>
       <c r="D424" s="5">
-        <v>44645</v>
+        <v>44798</v>
       </c>
       <c r="E424" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="425" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>7</v>
       </c>
       <c r="B425">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C425" s="5">
-        <v>44646</v>
+        <v>44713</v>
       </c>
       <c r="D425" s="5">
-        <v>44646</v>
-      </c>
-      <c r="E425" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="426" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44714</v>
+      </c>
+    </row>
+    <row r="426" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>7</v>
       </c>
       <c r="B426">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C426" s="5">
-        <v>44647</v>
+        <v>44715</v>
       </c>
       <c r="D426" s="5">
-        <v>44647</v>
-      </c>
-      <c r="E426" t="s">
-        <v>6</v>
+        <v>44715</v>
       </c>
     </row>
     <row r="427" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -7726,10 +7716,10 @@
         <v>10</v>
       </c>
       <c r="C427" s="5">
-        <v>44648</v>
+        <v>44728</v>
       </c>
       <c r="D427" s="5">
-        <v>44651</v>
+        <v>44865</v>
       </c>
       <c r="E427" t="s">
         <v>6</v>
@@ -7740,13 +7730,13 @@
         <v>5</v>
       </c>
       <c r="B428">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C428" s="5">
-        <v>44700</v>
+        <v>44743</v>
       </c>
       <c r="D428" s="5">
-        <v>44798</v>
+        <v>44746</v>
       </c>
       <c r="E428" t="s">
         <v>6</v>
@@ -7754,19 +7744,22 @@
     </row>
     <row r="429" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B429">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C429" s="5">
-        <v>44713</v>
+        <v>44743</v>
       </c>
       <c r="D429" s="5">
-        <v>44714</v>
-      </c>
-    </row>
-    <row r="430" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44765</v>
+      </c>
+      <c r="E429" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="430" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
         <v>7</v>
       </c>
@@ -7774,10 +7767,10 @@
         <v>11</v>
       </c>
       <c r="C430" s="5">
-        <v>44715</v>
+        <v>44743</v>
       </c>
       <c r="D430" s="5">
-        <v>44715</v>
+        <v>44743</v>
       </c>
     </row>
     <row r="431" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -7785,33 +7778,27 @@
         <v>7</v>
       </c>
       <c r="B431">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C431" s="5">
-        <v>44728</v>
+        <v>44743</v>
       </c>
       <c r="D431" s="5">
-        <v>44865</v>
-      </c>
-      <c r="E431" t="s">
-        <v>6</v>
+        <v>44834</v>
       </c>
     </row>
     <row r="432" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B432">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C432" s="5">
-        <v>44743</v>
+        <v>44744</v>
       </c>
       <c r="D432" s="5">
-        <v>44746</v>
-      </c>
-      <c r="E432" t="s">
-        <v>6</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="433" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -7819,19 +7806,19 @@
         <v>5</v>
       </c>
       <c r="B433">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C433" s="5">
-        <v>44743</v>
+        <v>44748</v>
       </c>
       <c r="D433" s="5">
-        <v>44765</v>
+        <v>44748</v>
       </c>
       <c r="E433" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="434" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
         <v>7</v>
       </c>
@@ -7839,27 +7826,31 @@
         <v>11</v>
       </c>
       <c r="C434" s="5">
-        <v>44743</v>
+        <v>44748</v>
       </c>
       <c r="D434" s="5">
-        <v>44743</v>
+        <v>44749</v>
       </c>
     </row>
     <row r="435" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B435">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C435" s="5">
-        <v>44743</v>
+        <v>44750</v>
       </c>
       <c r="D435" s="5">
-        <v>44834</v>
-      </c>
-    </row>
-    <row r="436" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <f>C435</f>
+        <v>44750</v>
+      </c>
+      <c r="E435" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="436" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
         <v>7</v>
       </c>
@@ -7867,44 +7858,45 @@
         <v>11</v>
       </c>
       <c r="C436" s="5">
-        <v>44744</v>
+        <v>44750</v>
       </c>
       <c r="D436" s="5">
-        <v>44744</v>
+        <v>44750</v>
       </c>
     </row>
     <row r="437" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B437">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C437" s="5">
-        <v>44748</v>
+        <v>44751</v>
       </c>
       <c r="D437" s="5">
-        <v>44748</v>
-      </c>
-      <c r="E437" t="s">
-        <v>6</v>
+        <v>44751</v>
       </c>
     </row>
     <row r="438" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B438">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C438" s="5">
-        <v>44748</v>
+        <v>44752</v>
       </c>
       <c r="D438" s="5">
-        <v>44749</v>
-      </c>
-    </row>
-    <row r="439" spans="1:5" x14ac:dyDescent="0.25">
+        <f>C438</f>
+        <v>44752</v>
+      </c>
+      <c r="E438" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="439" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
         <v>5</v>
       </c>
@@ -7912,11 +7904,11 @@
         <v>5</v>
       </c>
       <c r="C439" s="5">
-        <v>44750</v>
+        <v>44754</v>
       </c>
       <c r="D439" s="5">
         <f>C439</f>
-        <v>44750</v>
+        <v>44754</v>
       </c>
       <c r="E439" t="s">
         <v>6</v>
@@ -7924,51 +7916,57 @@
     </row>
     <row r="440" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B440">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C440" s="5">
-        <v>44750</v>
+        <v>44756</v>
       </c>
       <c r="D440" s="5">
-        <v>44750</v>
+        <f>C440</f>
+        <v>44756</v>
+      </c>
+      <c r="E440" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="441" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B441">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C441" s="5">
-        <v>44751</v>
+        <v>44756</v>
       </c>
       <c r="D441" s="5">
-        <v>44751</v>
-      </c>
-    </row>
-    <row r="442" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44758</v>
+      </c>
+      <c r="E441" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="442" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
         <v>5</v>
       </c>
       <c r="B442">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C442" s="5">
-        <v>44752</v>
+        <v>44756</v>
       </c>
       <c r="D442" s="5">
-        <f>C442</f>
-        <v>44752</v>
+        <v>44758</v>
       </c>
       <c r="E442" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="443" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
         <v>5</v>
       </c>
@@ -7976,17 +7974,17 @@
         <v>5</v>
       </c>
       <c r="C443" s="5">
-        <v>44754</v>
+        <v>44758</v>
       </c>
       <c r="D443" s="5">
         <f>C443</f>
-        <v>44754</v>
+        <v>44758</v>
       </c>
       <c r="E443" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="444" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
         <v>5</v>
       </c>
@@ -7994,11 +7992,11 @@
         <v>5</v>
       </c>
       <c r="C444" s="5">
-        <v>44756</v>
+        <v>44760</v>
       </c>
       <c r="D444" s="5">
         <f>C444</f>
-        <v>44756</v>
+        <v>44760</v>
       </c>
       <c r="E444" t="s">
         <v>6</v>
@@ -8009,13 +8007,14 @@
         <v>5</v>
       </c>
       <c r="B445">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C445" s="5">
-        <v>44756</v>
+        <v>44762</v>
       </c>
       <c r="D445" s="5">
-        <v>44758</v>
+        <f>C445</f>
+        <v>44762</v>
       </c>
       <c r="E445" t="s">
         <v>6</v>
@@ -8026,37 +8025,36 @@
         <v>5</v>
       </c>
       <c r="B446">
+        <v>7</v>
+      </c>
+      <c r="C446" s="5">
+        <v>44763</v>
+      </c>
+      <c r="D446" s="5">
+        <v>44765</v>
+      </c>
+      <c r="E446" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="447" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A447" t="s">
+        <v>5</v>
+      </c>
+      <c r="B447">
         <v>9</v>
       </c>
-      <c r="C446" s="5">
-        <v>44756</v>
-      </c>
-      <c r="D446" s="5">
-        <v>44758</v>
-      </c>
-      <c r="E446" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="447" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A447" t="s">
-        <v>5</v>
-      </c>
-      <c r="B447">
-        <v>5</v>
-      </c>
       <c r="C447" s="5">
-        <v>44758</v>
+        <v>44763</v>
       </c>
       <c r="D447" s="5">
-        <f>C447</f>
-        <v>44758</v>
+        <v>44765</v>
       </c>
       <c r="E447" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="448" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
         <v>5</v>
       </c>
@@ -8064,17 +8062,17 @@
         <v>5</v>
       </c>
       <c r="C448" s="5">
-        <v>44760</v>
+        <v>44764</v>
       </c>
       <c r="D448" s="5">
         <f>C448</f>
-        <v>44760</v>
+        <v>44764</v>
       </c>
       <c r="E448" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="449" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
         <v>5</v>
       </c>
@@ -8082,11 +8080,10 @@
         <v>5</v>
       </c>
       <c r="C449" s="5">
-        <v>44762</v>
+        <v>44766</v>
       </c>
       <c r="D449" s="5">
-        <f>C449</f>
-        <v>44762</v>
+        <v>44832</v>
       </c>
       <c r="E449" t="s">
         <v>6</v>
@@ -8097,13 +8094,13 @@
         <v>5</v>
       </c>
       <c r="B450">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C450" s="5">
-        <v>44763</v>
+        <v>44769</v>
       </c>
       <c r="D450" s="5">
-        <v>44765</v>
+        <v>44832</v>
       </c>
       <c r="E450" t="s">
         <v>6</v>
@@ -8114,119 +8111,106 @@
         <v>5</v>
       </c>
       <c r="B451">
+        <v>7</v>
+      </c>
+      <c r="C451" s="5">
+        <v>44770</v>
+      </c>
+      <c r="D451" s="5">
+        <v>44772</v>
+      </c>
+      <c r="E451" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="452" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A452" t="s">
+        <v>5</v>
+      </c>
+      <c r="B452">
         <v>9</v>
       </c>
-      <c r="C451" s="5">
-        <v>44763</v>
-      </c>
-      <c r="D451" s="5">
-        <v>44765</v>
-      </c>
-      <c r="E451" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="452" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A452" t="s">
-        <v>5</v>
-      </c>
-      <c r="B452">
-        <v>5</v>
-      </c>
       <c r="C452" s="5">
-        <v>44764</v>
+        <v>44770</v>
       </c>
       <c r="D452" s="5">
-        <f>C452</f>
-        <v>44764</v>
+        <v>44829</v>
       </c>
       <c r="E452" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="453" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B453">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="C453" s="5">
-        <v>44766</v>
+        <v>44774</v>
       </c>
       <c r="D453" s="5">
-        <v>44832</v>
-      </c>
-      <c r="E453" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="454" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44834</v>
+      </c>
+    </row>
+    <row r="454" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B454">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C454" s="5">
-        <v>44769</v>
+        <v>44776</v>
       </c>
       <c r="D454" s="5">
-        <v>44832</v>
-      </c>
-      <c r="E454" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="455" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44777</v>
+      </c>
+    </row>
+    <row r="455" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B455">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C455" s="5">
-        <v>44770</v>
+        <v>44778</v>
       </c>
       <c r="D455" s="5">
-        <v>44772</v>
-      </c>
-      <c r="E455" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="456" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44778</v>
+      </c>
+    </row>
+    <row r="456" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B456">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C456" s="5">
-        <v>44770</v>
+        <v>44779</v>
       </c>
       <c r="D456" s="5">
-        <v>44829</v>
-      </c>
-      <c r="E456" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="457" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44779</v>
+      </c>
+    </row>
+    <row r="457" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
         <v>7</v>
       </c>
       <c r="B457">
-        <v>81</v>
+        <v>11</v>
       </c>
       <c r="C457" s="5">
-        <v>44774</v>
+        <v>44783</v>
       </c>
       <c r="D457" s="5">
-        <v>44834</v>
-      </c>
-    </row>
-    <row r="458" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44784</v>
+      </c>
+    </row>
+    <row r="458" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
         <v>7</v>
       </c>
@@ -8234,13 +8218,13 @@
         <v>11</v>
       </c>
       <c r="C458" s="5">
-        <v>44776</v>
+        <v>44785</v>
       </c>
       <c r="D458" s="5">
-        <v>44777</v>
-      </c>
-    </row>
-    <row r="459" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44785</v>
+      </c>
+    </row>
+    <row r="459" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
         <v>7</v>
       </c>
@@ -8248,41 +8232,44 @@
         <v>11</v>
       </c>
       <c r="C459" s="5">
-        <v>44778</v>
+        <v>44786</v>
       </c>
       <c r="D459" s="5">
-        <v>44778</v>
+        <v>44786</v>
       </c>
     </row>
     <row r="460" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B460">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="C460" s="5">
-        <v>44779</v>
+        <v>44786</v>
       </c>
       <c r="D460" s="5">
-        <v>44779</v>
+        <v>44823</v>
       </c>
     </row>
     <row r="461" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B461">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C461" s="5">
-        <v>44783</v>
+        <v>44789</v>
       </c>
       <c r="D461" s="5">
-        <v>44784</v>
-      </c>
-    </row>
-    <row r="462" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44834</v>
+      </c>
+      <c r="E461" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="462" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
         <v>7</v>
       </c>
@@ -8290,13 +8277,13 @@
         <v>11</v>
       </c>
       <c r="C462" s="5">
-        <v>44785</v>
+        <v>44790</v>
       </c>
       <c r="D462" s="5">
-        <v>44785</v>
-      </c>
-    </row>
-    <row r="463" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44791</v>
+      </c>
+    </row>
+    <row r="463" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
         <v>7</v>
       </c>
@@ -8304,44 +8291,41 @@
         <v>11</v>
       </c>
       <c r="C463" s="5">
-        <v>44786</v>
+        <v>44792</v>
       </c>
       <c r="D463" s="5">
-        <v>44786</v>
-      </c>
-    </row>
-    <row r="464" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44792</v>
+      </c>
+    </row>
+    <row r="464" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B464">
-        <v>82</v>
+        <v>11</v>
       </c>
       <c r="C464" s="5">
-        <v>44786</v>
+        <v>44793</v>
       </c>
       <c r="D464" s="5">
-        <v>44823</v>
-      </c>
-    </row>
-    <row r="465" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44793</v>
+      </c>
+    </row>
+    <row r="465" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B465">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C465" s="5">
-        <v>44789</v>
+        <v>44794</v>
       </c>
       <c r="D465" s="5">
-        <v>44834</v>
-      </c>
-      <c r="E465" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="466" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44794</v>
+      </c>
+    </row>
+    <row r="466" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
         <v>7</v>
       </c>
@@ -8349,13 +8333,13 @@
         <v>11</v>
       </c>
       <c r="C466" s="5">
-        <v>44790</v>
+        <v>44795</v>
       </c>
       <c r="D466" s="5">
-        <v>44791</v>
-      </c>
-    </row>
-    <row r="467" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44798</v>
+      </c>
+    </row>
+    <row r="467" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
         <v>7</v>
       </c>
@@ -8363,13 +8347,13 @@
         <v>11</v>
       </c>
       <c r="C467" s="5">
-        <v>44792</v>
+        <v>44799</v>
       </c>
       <c r="D467" s="5">
-        <v>44792</v>
-      </c>
-    </row>
-    <row r="468" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44799</v>
+      </c>
+    </row>
+    <row r="468" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
         <v>7</v>
       </c>
@@ -8377,13 +8361,13 @@
         <v>11</v>
       </c>
       <c r="C468" s="5">
-        <v>44793</v>
+        <v>44800</v>
       </c>
       <c r="D468" s="5">
-        <v>44793</v>
-      </c>
-    </row>
-    <row r="469" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44800</v>
+      </c>
+    </row>
+    <row r="469" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
         <v>7</v>
       </c>
@@ -8391,13 +8375,13 @@
         <v>11</v>
       </c>
       <c r="C469" s="5">
-        <v>44794</v>
+        <v>44801</v>
       </c>
       <c r="D469" s="5">
-        <v>44794</v>
-      </c>
-    </row>
-    <row r="470" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44801</v>
+      </c>
+    </row>
+    <row r="470" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
         <v>7</v>
       </c>
@@ -8405,27 +8389,30 @@
         <v>11</v>
       </c>
       <c r="C470" s="5">
-        <v>44795</v>
+        <v>44802</v>
       </c>
       <c r="D470" s="5">
-        <v>44798</v>
+        <v>44805</v>
       </c>
     </row>
     <row r="471" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B471">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C471" s="5">
-        <v>44799</v>
+        <v>44804</v>
       </c>
       <c r="D471" s="5">
-        <v>44799</v>
-      </c>
-    </row>
-    <row r="472" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44834</v>
+      </c>
+      <c r="E471" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="472" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
         <v>7</v>
       </c>
@@ -8433,13 +8420,13 @@
         <v>11</v>
       </c>
       <c r="C472" s="5">
-        <v>44800</v>
+        <v>44806</v>
       </c>
       <c r="D472" s="5">
-        <v>44800</v>
-      </c>
-    </row>
-    <row r="473" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44806</v>
+      </c>
+    </row>
+    <row r="473" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
         <v>7</v>
       </c>
@@ -8447,13 +8434,13 @@
         <v>11</v>
       </c>
       <c r="C473" s="5">
-        <v>44801</v>
+        <v>44807</v>
       </c>
       <c r="D473" s="5">
-        <v>44801</v>
-      </c>
-    </row>
-    <row r="474" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44807</v>
+      </c>
+    </row>
+    <row r="474" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
         <v>7</v>
       </c>
@@ -8461,30 +8448,27 @@
         <v>11</v>
       </c>
       <c r="C474" s="5">
-        <v>44802</v>
+        <v>44808</v>
       </c>
       <c r="D474" s="5">
-        <v>44805</v>
-      </c>
-    </row>
-    <row r="475" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44809</v>
+      </c>
+    </row>
+    <row r="475" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A475" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B475">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C475" s="5">
-        <v>44804</v>
+        <v>44810</v>
       </c>
       <c r="D475" s="5">
-        <v>44834</v>
-      </c>
-      <c r="E475" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="476" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44812</v>
+      </c>
+    </row>
+    <row r="476" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
         <v>7</v>
       </c>
@@ -8492,13 +8476,13 @@
         <v>11</v>
       </c>
       <c r="C476" s="5">
-        <v>44806</v>
+        <v>44813</v>
       </c>
       <c r="D476" s="5">
-        <v>44806</v>
-      </c>
-    </row>
-    <row r="477" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44813</v>
+      </c>
+    </row>
+    <row r="477" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
         <v>7</v>
       </c>
@@ -8506,13 +8490,13 @@
         <v>11</v>
       </c>
       <c r="C477" s="5">
-        <v>44807</v>
+        <v>44814</v>
       </c>
       <c r="D477" s="5">
-        <v>44807</v>
-      </c>
-    </row>
-    <row r="478" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44814</v>
+      </c>
+    </row>
+    <row r="478" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
         <v>7</v>
       </c>
@@ -8520,13 +8504,13 @@
         <v>11</v>
       </c>
       <c r="C478" s="5">
-        <v>44808</v>
+        <v>44815</v>
       </c>
       <c r="D478" s="5">
-        <v>44809</v>
-      </c>
-    </row>
-    <row r="479" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44815</v>
+      </c>
+    </row>
+    <row r="479" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A479" t="s">
         <v>7</v>
       </c>
@@ -8534,13 +8518,13 @@
         <v>11</v>
       </c>
       <c r="C479" s="5">
-        <v>44810</v>
+        <v>44816</v>
       </c>
       <c r="D479" s="5">
-        <v>44812</v>
-      </c>
-    </row>
-    <row r="480" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44819</v>
+      </c>
+    </row>
+    <row r="480" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
         <v>7</v>
       </c>
@@ -8548,13 +8532,13 @@
         <v>11</v>
       </c>
       <c r="C480" s="5">
-        <v>44813</v>
+        <v>44820</v>
       </c>
       <c r="D480" s="5">
-        <v>44813</v>
-      </c>
-    </row>
-    <row r="481" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44820</v>
+      </c>
+    </row>
+    <row r="481" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
         <v>7</v>
       </c>
@@ -8562,13 +8546,13 @@
         <v>11</v>
       </c>
       <c r="C481" s="5">
-        <v>44814</v>
+        <v>44821</v>
       </c>
       <c r="D481" s="5">
-        <v>44814</v>
-      </c>
-    </row>
-    <row r="482" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44821</v>
+      </c>
+    </row>
+    <row r="482" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
         <v>7</v>
       </c>
@@ -8576,13 +8560,13 @@
         <v>11</v>
       </c>
       <c r="C482" s="5">
-        <v>44815</v>
+        <v>44822</v>
       </c>
       <c r="D482" s="5">
-        <v>44815</v>
-      </c>
-    </row>
-    <row r="483" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44822</v>
+      </c>
+    </row>
+    <row r="483" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
         <v>7</v>
       </c>
@@ -8590,13 +8574,13 @@
         <v>11</v>
       </c>
       <c r="C483" s="5">
-        <v>44816</v>
+        <v>44823</v>
       </c>
       <c r="D483" s="5">
-        <v>44819</v>
-      </c>
-    </row>
-    <row r="484" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44826</v>
+      </c>
+    </row>
+    <row r="484" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
         <v>7</v>
       </c>
@@ -8604,13 +8588,13 @@
         <v>11</v>
       </c>
       <c r="C484" s="5">
-        <v>44820</v>
+        <v>44827</v>
       </c>
       <c r="D484" s="5">
-        <v>44820</v>
-      </c>
-    </row>
-    <row r="485" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44827</v>
+      </c>
+    </row>
+    <row r="485" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
         <v>7</v>
       </c>
@@ -8618,13 +8602,13 @@
         <v>11</v>
       </c>
       <c r="C485" s="5">
-        <v>44821</v>
+        <v>44828</v>
       </c>
       <c r="D485" s="5">
-        <v>44821</v>
-      </c>
-    </row>
-    <row r="486" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44828</v>
+      </c>
+    </row>
+    <row r="486" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
         <v>7</v>
       </c>
@@ -8632,13 +8616,13 @@
         <v>11</v>
       </c>
       <c r="C486" s="5">
-        <v>44822</v>
+        <v>44829</v>
       </c>
       <c r="D486" s="5">
-        <v>44822</v>
-      </c>
-    </row>
-    <row r="487" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44829</v>
+      </c>
+    </row>
+    <row r="487" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
         <v>7</v>
       </c>
@@ -8646,13 +8630,13 @@
         <v>11</v>
       </c>
       <c r="C487" s="5">
-        <v>44823</v>
+        <v>44830</v>
       </c>
       <c r="D487" s="5">
-        <v>44826</v>
-      </c>
-    </row>
-    <row r="488" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44833</v>
+      </c>
+    </row>
+    <row r="488" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
         <v>7</v>
       </c>
@@ -8660,13 +8644,13 @@
         <v>11</v>
       </c>
       <c r="C488" s="5">
-        <v>44827</v>
+        <v>44834</v>
       </c>
       <c r="D488" s="5">
-        <v>44827</v>
-      </c>
-    </row>
-    <row r="489" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44834</v>
+      </c>
+    </row>
+    <row r="489" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
         <v>7</v>
       </c>
@@ -8674,10 +8658,10 @@
         <v>11</v>
       </c>
       <c r="C489" s="5">
-        <v>44828</v>
+        <v>44835</v>
       </c>
       <c r="D489" s="5">
-        <v>44828</v>
+        <v>44865</v>
       </c>
     </row>
     <row r="490" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8685,27 +8669,30 @@
         <v>7</v>
       </c>
       <c r="B490">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C490" s="5">
-        <v>44829</v>
+        <v>44835</v>
       </c>
       <c r="D490" s="5">
-        <v>44829</v>
+        <v>44865</v>
       </c>
     </row>
     <row r="491" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B491">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C491" s="5">
-        <v>44830</v>
+        <v>44835</v>
       </c>
       <c r="D491" s="5">
-        <v>44833</v>
+        <v>45046</v>
+      </c>
+      <c r="E491" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="492" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8713,172 +8700,28 @@
         <v>7</v>
       </c>
       <c r="B492">
-        <v>11</v>
+        <v>81</v>
       </c>
       <c r="C492" s="5">
-        <v>44834</v>
+        <v>44835</v>
       </c>
       <c r="D492" s="5">
-        <v>44834</v>
-      </c>
-    </row>
-    <row r="493" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A493" t="s">
-        <v>7</v>
-      </c>
-      <c r="B493">
-        <v>11</v>
-      </c>
-      <c r="C493" s="5">
-        <v>44835</v>
-      </c>
-      <c r="D493" s="5">
-        <v>44865</v>
-      </c>
-    </row>
-    <row r="494" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A494" t="s">
-        <v>7</v>
-      </c>
-      <c r="B494">
-        <v>11</v>
-      </c>
-      <c r="C494" s="5">
-        <v>44835</v>
-      </c>
-      <c r="D494" s="5">
-        <v>44835</v>
-      </c>
-    </row>
-    <row r="495" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A495" t="s">
-        <v>7</v>
-      </c>
-      <c r="B495">
-        <v>12</v>
-      </c>
-      <c r="C495" s="5">
-        <v>44835</v>
-      </c>
-      <c r="D495" s="5">
-        <v>44865</v>
-      </c>
-    </row>
-    <row r="496" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A496" t="s">
-        <v>5</v>
-      </c>
-      <c r="B496">
-        <v>13</v>
-      </c>
-      <c r="C496" s="5">
-        <v>44835</v>
-      </c>
-      <c r="D496" s="5">
-        <v>45046</v>
-      </c>
-      <c r="E496" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="497" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A497" t="s">
-        <v>7</v>
-      </c>
-      <c r="B497">
-        <v>81</v>
-      </c>
-      <c r="C497" s="5">
-        <v>44835</v>
-      </c>
-      <c r="D497" s="5">
         <v>44843</v>
       </c>
     </row>
-    <row r="498" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A498" t="s">
-        <v>7</v>
-      </c>
-      <c r="B498">
-        <v>11</v>
-      </c>
-      <c r="C498" s="5">
-        <v>44836</v>
-      </c>
-      <c r="D498" s="5">
-        <v>44836</v>
-      </c>
-    </row>
-    <row r="499" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A499" t="s">
-        <v>7</v>
-      </c>
-      <c r="B499">
-        <v>11</v>
-      </c>
-      <c r="C499" s="5">
-        <v>44837</v>
-      </c>
-      <c r="D499" s="5">
-        <v>44840</v>
-      </c>
-    </row>
-    <row r="500" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A500" t="s">
-        <v>7</v>
-      </c>
-      <c r="B500">
-        <v>11</v>
-      </c>
-      <c r="C500" s="5">
-        <v>44841</v>
-      </c>
-      <c r="D500" s="5">
-        <v>44841</v>
-      </c>
-    </row>
-    <row r="501" spans="1:4" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A501" t="s">
-        <v>7</v>
-      </c>
-      <c r="B501">
-        <v>11</v>
-      </c>
-      <c r="C501" s="5">
-        <v>44842</v>
-      </c>
-      <c r="D501" s="5">
-        <v>44842</v>
-      </c>
-    </row>
-    <row r="502" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A502" t="s">
-        <v>7</v>
-      </c>
-      <c r="B502">
-        <v>11</v>
-      </c>
-      <c r="C502" s="5">
-        <v>44843</v>
-      </c>
-      <c r="D502" s="5">
-        <v>44843</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:E502" xr:uid="{9536AF9F-EFE7-469A-8B3B-7525E4B6BE61}">
+  <autoFilter ref="A1:E492" xr:uid="{9536AF9F-EFE7-469A-8B3B-7525E4B6BE61}">
     <filterColumn colId="1">
       <filters>
-        <filter val="5"/>
+        <filter val="11"/>
       </filters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E43">
-      <sortCondition ref="B2:B502"/>
-      <sortCondition ref="C2:C502"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:E449">
+      <sortCondition ref="C264:C492"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E502">
-    <sortCondition ref="C207:C502"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E492">
+    <sortCondition ref="C207:C492"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8900,6 +8743,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DE9114A9D0DECB469CD3434F7556ACE4" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d7c6d40c49ba7a98dce712687acf420b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="62120a19-a38a-4c78-8e86-03b65bdcf4fa" xmlns:ns3="671c5c8a-d1dd-40a7-bcfd-3ed591bedb5d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5f8f7844aaab423fe57564514e62d9bb" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -9139,15 +8991,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37A00794-6F8A-440F-8D17-1F18CC3F357B}">
   <ds:schemaRefs>
@@ -9161,6 +9004,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{902BFF43-0B71-4183-AE7E-FA994EED3F0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EFEA11F-658A-4460-92CA-EE713A46DF11}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9178,12 +9029,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{902BFF43-0B71-4183-AE7E-FA994EED3F0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
regulation fixes: area 5, oct 2015; area 10, june 2018; added a script to dump non-retention catch from daily crc estimates
</commit_message>
<xml_diff>
--- a/data/sources/coho_regulations.xlsx
+++ b/data/sources/coho_regulations.xlsx
@@ -5,18 +5,18 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\sport_harvest\sport\sport_harvest_estimator\data\sources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/tyler_garber_dfw_wa_gov/Documents/sport_harvest/sport/sport_harvest_estimator/data/sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F960066-A2E8-41E3-8CB8-A4E7D7F70CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{3F960066-A2E8-41E3-8CB8-A4E7D7F70CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDE6AF75-02D0-4D23-BAA2-3895173C3981}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29325" yWindow="4005" windowWidth="19185" windowHeight="10185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="coho_regulations" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">coho_regulations!$A$1:$E$492</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">coho_regulations!$A$1:$E$493</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="8">
   <si>
     <t>regulation_type_code</t>
   </si>
@@ -471,11 +471,11 @@
   <sheetPr codeName="Sheet1" filterMode="1">
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:E492"/>
+  <dimension ref="A1:E493"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A245" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D359" sqref="D359"/>
+      <pane ySplit="1" topLeftCell="A250" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C271" sqref="C271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,7 +521,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -589,7 +589,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -776,7 +776,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -878,7 +878,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -929,7 +929,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>7</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>7</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>7</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>7</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>7</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>7</v>
       </c>
@@ -1830,7 +1830,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>7</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>7</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>7</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="103" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>7</v>
       </c>
@@ -2527,7 +2527,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>7</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>7</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="129" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>7</v>
       </c>
@@ -2986,7 +2986,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>7</v>
       </c>
@@ -3054,7 +3054,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>7</v>
       </c>
@@ -3122,7 +3122,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="156" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>7</v>
       </c>
@@ -3360,7 +3360,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>7</v>
       </c>
@@ -3462,7 +3462,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>7</v>
       </c>
@@ -3530,7 +3530,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="180" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>7</v>
       </c>
@@ -3802,7 +3802,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>7</v>
       </c>
@@ -3887,7 +3887,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>7</v>
       </c>
@@ -3955,7 +3955,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="205" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>7</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>7</v>
       </c>
@@ -4261,7 +4261,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>7</v>
       </c>
@@ -4346,7 +4346,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="228" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>7</v>
       </c>
@@ -4567,7 +4567,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>7</v>
       </c>
@@ -4635,7 +4635,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>7</v>
       </c>
@@ -4720,7 +4720,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="250" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>7</v>
       </c>
@@ -4924,7 +4924,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>7</v>
       </c>
@@ -4992,7 +4992,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>7</v>
       </c>
@@ -5077,7 +5077,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="271" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>7</v>
       </c>
@@ -5298,7 +5298,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>7</v>
       </c>
@@ -5349,7 +5349,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>7</v>
       </c>
@@ -5417,7 +5417,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="291" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>7</v>
       </c>
@@ -5663,7 +5663,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>7</v>
       </c>
@@ -5731,7 +5731,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="310" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>7</v>
       </c>
@@ -5782,7 +5782,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>7</v>
       </c>
@@ -5824,13 +5824,10 @@
         <v>5</v>
       </c>
       <c r="C315" s="5">
-        <v>42416</v>
+        <v>42278</v>
       </c>
       <c r="D315" s="5">
-        <v>42490</v>
-      </c>
-      <c r="E315" t="s">
-        <v>6</v>
+        <v>42308</v>
       </c>
     </row>
     <row r="316" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -5838,13 +5835,13 @@
         <v>7</v>
       </c>
       <c r="B316">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C316" s="5">
-        <v>42552</v>
+        <v>42416</v>
       </c>
       <c r="D316" s="5">
-        <v>42674</v>
+        <v>42490</v>
       </c>
       <c r="E316" t="s">
         <v>6</v>
@@ -5852,16 +5849,16 @@
     </row>
     <row r="317" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B317">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C317" s="5">
-        <v>42644</v>
+        <v>42552</v>
       </c>
       <c r="D317" s="5">
-        <v>42664</v>
+        <v>42674</v>
       </c>
       <c r="E317" t="s">
         <v>6</v>
@@ -5869,16 +5866,16 @@
     </row>
     <row r="318" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B318">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C318" s="5">
-        <v>42675</v>
+        <v>42644</v>
       </c>
       <c r="D318" s="5">
-        <v>42855</v>
+        <v>42664</v>
       </c>
       <c r="E318" t="s">
         <v>6</v>
@@ -5886,33 +5883,33 @@
     </row>
     <row r="319" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B319">
+        <v>12</v>
+      </c>
+      <c r="C319" s="5">
+        <v>42675</v>
+      </c>
+      <c r="D319" s="5">
+        <v>42855</v>
+      </c>
+      <c r="E319" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="320" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
+        <v>5</v>
+      </c>
+      <c r="B320">
         <v>13</v>
       </c>
-      <c r="C319" s="5">
+      <c r="C320" s="5">
         <v>42856</v>
       </c>
-      <c r="D319" s="5">
+      <c r="D320" s="5">
         <v>43008</v>
-      </c>
-      <c r="E319" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A320" t="s">
-        <v>7</v>
-      </c>
-      <c r="B320">
-        <v>11</v>
-      </c>
-      <c r="C320" s="5">
-        <v>42887</v>
-      </c>
-      <c r="D320" s="5">
-        <v>43039</v>
       </c>
       <c r="E320" t="s">
         <v>6</v>
@@ -5920,16 +5917,16 @@
     </row>
     <row r="321" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B321">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C321" s="5">
-        <v>42917</v>
+        <v>42887</v>
       </c>
       <c r="D321" s="5">
-        <v>42978</v>
+        <v>43039</v>
       </c>
       <c r="E321" t="s">
         <v>6</v>
@@ -5940,13 +5937,13 @@
         <v>5</v>
       </c>
       <c r="B322">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C322" s="5">
         <v>42917</v>
       </c>
       <c r="D322" s="5">
-        <v>42962</v>
+        <v>42978</v>
       </c>
       <c r="E322" t="s">
         <v>6</v>
@@ -5954,16 +5951,16 @@
     </row>
     <row r="323" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B323">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C323" s="5">
         <v>42917</v>
       </c>
       <c r="D323" s="5">
-        <v>43008</v>
+        <v>42962</v>
       </c>
       <c r="E323" t="s">
         <v>6</v>
@@ -5974,13 +5971,13 @@
         <v>7</v>
       </c>
       <c r="B324">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C324" s="5">
         <v>42917</v>
       </c>
       <c r="D324" s="5">
-        <v>43069</v>
+        <v>43008</v>
       </c>
       <c r="E324" t="s">
         <v>6</v>
@@ -5988,16 +5985,16 @@
     </row>
     <row r="325" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B325">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C325" s="5">
-        <v>42932</v>
+        <v>42917</v>
       </c>
       <c r="D325" s="5">
-        <v>42982</v>
+        <v>43069</v>
       </c>
       <c r="E325" t="s">
         <v>6</v>
@@ -6008,30 +6005,30 @@
         <v>5</v>
       </c>
       <c r="B326">
+        <v>9</v>
+      </c>
+      <c r="C326" s="5">
+        <v>42932</v>
+      </c>
+      <c r="D326" s="5">
+        <v>42982</v>
+      </c>
+      <c r="E326" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
+        <v>5</v>
+      </c>
+      <c r="B327">
         <v>10</v>
       </c>
-      <c r="C326" s="5">
+      <c r="C327" s="5">
         <v>42917</v>
       </c>
-      <c r="D326" s="5">
+      <c r="D327" s="5">
         <v>43159</v>
-      </c>
-      <c r="E326" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="327" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A327" t="s">
-        <v>5</v>
-      </c>
-      <c r="B327">
-        <v>82</v>
-      </c>
-      <c r="C327" s="5">
-        <v>42948</v>
-      </c>
-      <c r="D327" s="5">
-        <v>42982</v>
       </c>
       <c r="E327" t="s">
         <v>6</v>
@@ -6042,27 +6039,27 @@
         <v>5</v>
       </c>
       <c r="B328">
+        <v>82</v>
+      </c>
+      <c r="C328" s="5">
+        <v>42948</v>
+      </c>
+      <c r="D328" s="5">
+        <v>42982</v>
+      </c>
+      <c r="E328" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="329" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
+        <v>5</v>
+      </c>
+      <c r="B329">
         <v>13</v>
       </c>
-      <c r="C328" s="5">
+      <c r="C329" s="5">
         <v>43009</v>
-      </c>
-      <c r="D328" s="5">
-        <v>43220</v>
-      </c>
-      <c r="E328" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A329" t="s">
-        <v>5</v>
-      </c>
-      <c r="B329">
-        <v>11</v>
-      </c>
-      <c r="C329" s="5">
-        <v>43040</v>
       </c>
       <c r="D329" s="5">
         <v>43220</v>
@@ -6073,13 +6070,13 @@
     </row>
     <row r="330" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B330">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C330" s="5">
-        <v>43070</v>
+        <v>43040</v>
       </c>
       <c r="D330" s="5">
         <v>43220</v>
@@ -6090,33 +6087,33 @@
     </row>
     <row r="331" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B331">
+        <v>12</v>
+      </c>
+      <c r="C331" s="5">
+        <v>43070</v>
+      </c>
+      <c r="D331" s="5">
+        <v>43220</v>
+      </c>
+      <c r="E331" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="332" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
+        <v>5</v>
+      </c>
+      <c r="B332">
         <v>13</v>
       </c>
-      <c r="C331" s="5">
+      <c r="C332" s="5">
         <v>43221</v>
       </c>
-      <c r="D331" s="5">
+      <c r="D332" s="5">
         <v>43373</v>
-      </c>
-      <c r="E331" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A332" t="s">
-        <v>7</v>
-      </c>
-      <c r="B332">
-        <v>11</v>
-      </c>
-      <c r="C332" s="5">
-        <v>43252</v>
-      </c>
-      <c r="D332" s="5">
-        <v>43297</v>
       </c>
       <c r="E332" t="s">
         <v>6</v>
@@ -6124,16 +6121,16 @@
     </row>
     <row r="333" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B333">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C333" s="5">
-        <v>43282</v>
+        <v>43252</v>
       </c>
       <c r="D333" s="5">
-        <v>43373</v>
+        <v>43297</v>
       </c>
       <c r="E333" t="s">
         <v>6</v>
@@ -6144,7 +6141,7 @@
         <v>5</v>
       </c>
       <c r="B334">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C334" s="5">
         <v>43282</v>
@@ -6158,10 +6155,10 @@
     </row>
     <row r="335" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B335">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C335" s="5">
         <v>43282</v>
@@ -6178,30 +6175,30 @@
         <v>7</v>
       </c>
       <c r="B336">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C336" s="5">
         <v>43282</v>
       </c>
       <c r="D336" s="5">
+        <v>43373</v>
+      </c>
+      <c r="E336" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
+        <v>7</v>
+      </c>
+      <c r="B337">
+        <v>10</v>
+      </c>
+      <c r="C337" s="5">
+        <v>43252</v>
+      </c>
+      <c r="D337" s="5">
         <v>43419</v>
-      </c>
-      <c r="E336" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="337" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A337" t="s">
-        <v>7</v>
-      </c>
-      <c r="B337">
-        <v>12</v>
-      </c>
-      <c r="C337" s="5">
-        <v>43282</v>
-      </c>
-      <c r="D337" s="5">
-        <v>43404</v>
       </c>
       <c r="E337" t="s">
         <v>6</v>
@@ -6209,39 +6206,39 @@
     </row>
     <row r="338" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B338">
+        <v>12</v>
+      </c>
+      <c r="C338" s="5">
+        <v>43282</v>
+      </c>
+      <c r="D338" s="5">
+        <v>43404</v>
+      </c>
+      <c r="E338" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="339" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A339" t="s">
+        <v>5</v>
+      </c>
+      <c r="B339">
         <v>9</v>
       </c>
-      <c r="C338" s="5">
+      <c r="C339" s="5">
         <v>43297</v>
       </c>
-      <c r="D338" s="5">
+      <c r="D339" s="5">
         <v>43373</v>
       </c>
-      <c r="E338" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A339" t="s">
-        <v>7</v>
-      </c>
-      <c r="B339">
-        <v>11</v>
-      </c>
-      <c r="C339" s="5">
-        <v>43301</v>
-      </c>
-      <c r="D339" s="5">
-        <v>43304</v>
-      </c>
       <c r="E339" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>7</v>
       </c>
@@ -6249,16 +6246,16 @@
         <v>11</v>
       </c>
       <c r="C340" s="5">
-        <v>43308</v>
+        <v>43301</v>
       </c>
       <c r="D340" s="5">
-        <v>43311</v>
+        <v>43304</v>
       </c>
       <c r="E340" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>7</v>
       </c>
@@ -6266,10 +6263,10 @@
         <v>11</v>
       </c>
       <c r="C341" s="5">
-        <v>43312</v>
+        <v>43308</v>
       </c>
       <c r="D341" s="5">
-        <v>43373</v>
+        <v>43311</v>
       </c>
       <c r="E341" t="s">
         <v>6</v>
@@ -6280,10 +6277,10 @@
         <v>7</v>
       </c>
       <c r="B342">
-        <v>81</v>
+        <v>11</v>
       </c>
       <c r="C342" s="5">
-        <v>43313</v>
+        <v>43312</v>
       </c>
       <c r="D342" s="5">
         <v>43373</v>
@@ -6297,13 +6294,13 @@
         <v>7</v>
       </c>
       <c r="B343">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C343" s="5">
         <v>43313</v>
       </c>
       <c r="D343" s="5">
-        <v>43366</v>
+        <v>43373</v>
       </c>
       <c r="E343" t="s">
         <v>6</v>
@@ -6311,16 +6308,16 @@
     </row>
     <row r="344" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B344">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="C344" s="5">
-        <v>43374</v>
+        <v>43313</v>
       </c>
       <c r="D344" s="5">
-        <v>43585</v>
+        <v>43366</v>
       </c>
       <c r="E344" t="s">
         <v>6</v>
@@ -6328,13 +6325,13 @@
     </row>
     <row r="345" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B345">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C345" s="5">
-        <v>43405</v>
+        <v>43374</v>
       </c>
       <c r="D345" s="5">
         <v>43585</v>
@@ -6343,15 +6340,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>7</v>
       </c>
       <c r="B346">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C346" s="5">
-        <v>43374</v>
+        <v>43405</v>
       </c>
       <c r="D346" s="5">
         <v>43585</v>
@@ -6365,30 +6362,30 @@
         <v>7</v>
       </c>
       <c r="B347">
+        <v>11</v>
+      </c>
+      <c r="C347" s="5">
+        <v>43374</v>
+      </c>
+      <c r="D347" s="5">
+        <v>43585</v>
+      </c>
+      <c r="E347" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A348" t="s">
+        <v>7</v>
+      </c>
+      <c r="B348">
         <v>10</v>
       </c>
-      <c r="C347" s="5">
+      <c r="C348" s="5">
         <v>43466</v>
       </c>
-      <c r="D347" s="5">
+      <c r="D348" s="5">
         <v>43555</v>
-      </c>
-      <c r="E347" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="348" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A348" t="s">
-        <v>5</v>
-      </c>
-      <c r="B348">
-        <v>6</v>
-      </c>
-      <c r="C348" s="5">
-        <v>43497</v>
-      </c>
-      <c r="D348" s="5">
-        <v>43570</v>
       </c>
       <c r="E348" t="s">
         <v>6</v>
@@ -6399,13 +6396,13 @@
         <v>5</v>
       </c>
       <c r="B349">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C349" s="5">
-        <v>43512</v>
+        <v>43497</v>
       </c>
       <c r="D349" s="5">
-        <v>43585</v>
+        <v>43570</v>
       </c>
       <c r="E349" t="s">
         <v>6</v>
@@ -6416,13 +6413,13 @@
         <v>5</v>
       </c>
       <c r="B350">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C350" s="5">
-        <v>43586</v>
+        <v>43512</v>
       </c>
       <c r="D350" s="5">
-        <v>43738</v>
+        <v>43585</v>
       </c>
       <c r="E350" t="s">
         <v>6</v>
@@ -6430,33 +6427,33 @@
     </row>
     <row r="351" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B351">
+        <v>13</v>
+      </c>
+      <c r="C351" s="5">
+        <v>43586</v>
+      </c>
+      <c r="D351" s="5">
+        <v>43738</v>
+      </c>
+      <c r="E351" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
+        <v>7</v>
+      </c>
+      <c r="B352">
         <v>10</v>
       </c>
-      <c r="C351" s="5">
+      <c r="C352" s="5">
         <v>43617</v>
       </c>
-      <c r="D351" s="5">
+      <c r="D352" s="5">
         <v>43784</v>
-      </c>
-      <c r="E351" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="352" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A352" t="s">
-        <v>5</v>
-      </c>
-      <c r="B352">
-        <v>5</v>
-      </c>
-      <c r="C352" s="5">
-        <v>43647</v>
-      </c>
-      <c r="D352" s="5">
-        <v>43738</v>
       </c>
       <c r="E352" t="s">
         <v>6</v>
@@ -6467,7 +6464,7 @@
         <v>5</v>
       </c>
       <c r="B353">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C353" s="5">
         <v>43647</v>
@@ -6481,33 +6478,33 @@
     </row>
     <row r="354" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B354">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C354" s="5">
         <v>43647</v>
       </c>
       <c r="D354" s="5">
-        <v>43677</v>
+        <v>43738</v>
       </c>
       <c r="E354" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>7</v>
       </c>
       <c r="B355">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C355" s="5">
         <v>43647</v>
       </c>
       <c r="D355" s="5">
-        <v>43649</v>
+        <v>43677</v>
       </c>
       <c r="E355" t="s">
         <v>6</v>
@@ -6518,36 +6515,36 @@
         <v>7</v>
       </c>
       <c r="B356">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C356" s="5">
         <v>43647</v>
       </c>
       <c r="D356" s="5">
+        <v>43649</v>
+      </c>
+      <c r="E356" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="357" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A357" t="s">
+        <v>7</v>
+      </c>
+      <c r="B357">
+        <v>12</v>
+      </c>
+      <c r="C357" s="5">
+        <v>43647</v>
+      </c>
+      <c r="D357" s="5">
         <v>43769</v>
       </c>
-      <c r="E356" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A357" t="s">
-        <v>7</v>
-      </c>
-      <c r="B357">
-        <v>11</v>
-      </c>
-      <c r="C357" s="5">
-        <v>43652</v>
-      </c>
-      <c r="D357" s="5">
-        <v>43656</v>
-      </c>
       <c r="E357" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>7</v>
       </c>
@@ -6555,16 +6552,16 @@
         <v>11</v>
       </c>
       <c r="C358" s="5">
-        <v>43659</v>
+        <v>43652</v>
       </c>
       <c r="D358" s="5">
-        <v>43663</v>
+        <v>43656</v>
       </c>
       <c r="E358" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>7</v>
       </c>
@@ -6572,10 +6569,10 @@
         <v>11</v>
       </c>
       <c r="C359" s="5">
-        <v>43666</v>
+        <v>43659</v>
       </c>
       <c r="D359" s="5">
-        <v>43670</v>
+        <v>43663</v>
       </c>
       <c r="E359" t="s">
         <v>6</v>
@@ -6583,33 +6580,33 @@
     </row>
     <row r="360" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B360">
+        <v>11</v>
+      </c>
+      <c r="C360" s="5">
+        <v>43666</v>
+      </c>
+      <c r="D360" s="5">
+        <v>43670</v>
+      </c>
+      <c r="E360" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="361" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A361" t="s">
+        <v>5</v>
+      </c>
+      <c r="B361">
         <v>9</v>
       </c>
-      <c r="C360" s="5">
+      <c r="C361" s="5">
         <v>43671</v>
       </c>
-      <c r="D360" s="5">
+      <c r="D361" s="5">
         <v>43738</v>
-      </c>
-      <c r="E360" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A361" t="s">
-        <v>7</v>
-      </c>
-      <c r="B361">
-        <v>11</v>
-      </c>
-      <c r="C361" s="5">
-        <v>43673</v>
-      </c>
-      <c r="D361" s="5">
-        <v>43677</v>
       </c>
       <c r="E361" t="s">
         <v>6</v>
@@ -6620,36 +6617,36 @@
         <v>7</v>
       </c>
       <c r="B362">
+        <v>11</v>
+      </c>
+      <c r="C362" s="5">
+        <v>43673</v>
+      </c>
+      <c r="D362" s="5">
+        <v>43677</v>
+      </c>
+      <c r="E362" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="363" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A363" t="s">
+        <v>7</v>
+      </c>
+      <c r="B363">
         <v>81</v>
       </c>
-      <c r="C362" s="5">
+      <c r="C363" s="5">
         <v>43678</v>
       </c>
-      <c r="D362" s="5">
+      <c r="D363" s="5">
         <v>43769</v>
       </c>
-      <c r="E362" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A363" t="s">
-        <v>7</v>
-      </c>
-      <c r="B363">
-        <v>11</v>
-      </c>
-      <c r="C363" s="5">
-        <v>43680</v>
-      </c>
-      <c r="D363" s="5">
-        <v>43684</v>
-      </c>
       <c r="E363" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>7</v>
       </c>
@@ -6657,10 +6654,10 @@
         <v>11</v>
       </c>
       <c r="C364" s="5">
-        <v>43687</v>
+        <v>43680</v>
       </c>
       <c r="D364" s="5">
-        <v>43691</v>
+        <v>43684</v>
       </c>
       <c r="E364" t="s">
         <v>6</v>
@@ -6668,39 +6665,39 @@
     </row>
     <row r="365" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B365">
+        <v>11</v>
+      </c>
+      <c r="C365" s="5">
+        <v>43687</v>
+      </c>
+      <c r="D365" s="5">
+        <v>43691</v>
+      </c>
+      <c r="E365" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="366" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A366" t="s">
+        <v>5</v>
+      </c>
+      <c r="B366">
         <v>82</v>
       </c>
-      <c r="C365" s="5">
+      <c r="C366" s="5">
         <v>43693</v>
       </c>
-      <c r="D365" s="5">
+      <c r="D366" s="5">
         <v>43723</v>
       </c>
-      <c r="E365" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A366" t="s">
-        <v>7</v>
-      </c>
-      <c r="B366">
-        <v>11</v>
-      </c>
-      <c r="C366" s="5">
-        <v>43694</v>
-      </c>
-      <c r="D366" s="5">
-        <v>43698</v>
-      </c>
       <c r="E366" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>7</v>
       </c>
@@ -6708,16 +6705,16 @@
         <v>11</v>
       </c>
       <c r="C367" s="5">
-        <v>43701</v>
+        <v>43694</v>
       </c>
       <c r="D367" s="5">
-        <v>43702</v>
+        <v>43698</v>
       </c>
       <c r="E367" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>7</v>
       </c>
@@ -6725,10 +6722,10 @@
         <v>11</v>
       </c>
       <c r="C368" s="5">
-        <v>43703</v>
+        <v>43701</v>
       </c>
       <c r="D368" s="5">
-        <v>43738</v>
+        <v>43702</v>
       </c>
       <c r="E368" t="s">
         <v>6</v>
@@ -6739,10 +6736,10 @@
         <v>7</v>
       </c>
       <c r="B369">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C369" s="5">
-        <v>43709</v>
+        <v>43703</v>
       </c>
       <c r="D369" s="5">
         <v>43738</v>
@@ -6753,16 +6750,16 @@
     </row>
     <row r="370" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B370">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C370" s="5">
-        <v>43739</v>
+        <v>43709</v>
       </c>
       <c r="D370" s="5">
-        <v>43914</v>
+        <v>43738</v>
       </c>
       <c r="E370" t="s">
         <v>6</v>
@@ -6770,16 +6767,16 @@
     </row>
     <row r="371" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B371">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C371" s="5">
-        <v>43770</v>
+        <v>43739</v>
       </c>
       <c r="D371" s="5">
-        <v>43951</v>
+        <v>43914</v>
       </c>
       <c r="E371" t="s">
         <v>6</v>
@@ -6790,13 +6787,13 @@
         <v>7</v>
       </c>
       <c r="B372">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C372" s="5">
-        <v>43831</v>
+        <v>43770</v>
       </c>
       <c r="D372" s="5">
-        <v>43914</v>
+        <v>43951</v>
       </c>
       <c r="E372" t="s">
         <v>6</v>
@@ -6807,13 +6804,13 @@
         <v>7</v>
       </c>
       <c r="B373">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C373" s="5">
         <v>43831</v>
       </c>
       <c r="D373" s="5">
-        <v>43951</v>
+        <v>43914</v>
       </c>
       <c r="E373" t="s">
         <v>6</v>
@@ -6821,16 +6818,16 @@
     </row>
     <row r="374" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B374">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C374" s="5">
-        <v>43862</v>
+        <v>43831</v>
       </c>
       <c r="D374" s="5">
-        <v>43914</v>
+        <v>43951</v>
       </c>
       <c r="E374" t="s">
         <v>6</v>
@@ -6841,10 +6838,10 @@
         <v>5</v>
       </c>
       <c r="B375">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C375" s="5">
-        <v>43891</v>
+        <v>43862</v>
       </c>
       <c r="D375" s="5">
         <v>43914</v>
@@ -6858,7 +6855,7 @@
         <v>5</v>
       </c>
       <c r="B376">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C376" s="5">
         <v>43891</v>
@@ -6875,13 +6872,13 @@
         <v>5</v>
       </c>
       <c r="B377">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C377" s="5">
-        <v>43958</v>
+        <v>43891</v>
       </c>
       <c r="D377" s="5">
-        <v>44104</v>
+        <v>43914</v>
       </c>
       <c r="E377" t="s">
         <v>6</v>
@@ -6889,33 +6886,33 @@
     </row>
     <row r="378" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B378">
+        <v>13</v>
+      </c>
+      <c r="C378" s="5">
+        <v>43958</v>
+      </c>
+      <c r="D378" s="5">
+        <v>44104</v>
+      </c>
+      <c r="E378" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A379" t="s">
+        <v>7</v>
+      </c>
+      <c r="B379">
         <v>10</v>
       </c>
-      <c r="C378" s="5">
+      <c r="C379" s="5">
         <v>43983</v>
       </c>
-      <c r="D378" s="5">
+      <c r="D379" s="5">
         <v>44150</v>
-      </c>
-      <c r="E378" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="379" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A379" t="s">
-        <v>5</v>
-      </c>
-      <c r="B379">
-        <v>5</v>
-      </c>
-      <c r="C379" s="5">
-        <v>44013</v>
-      </c>
-      <c r="D379" s="5">
-        <v>44104</v>
       </c>
       <c r="E379" t="s">
         <v>6</v>
@@ -6926,7 +6923,7 @@
         <v>5</v>
       </c>
       <c r="B380">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C380" s="5">
         <v>44013</v>
@@ -6940,10 +6937,10 @@
     </row>
     <row r="381" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B381">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C381" s="5">
         <v>44013</v>
@@ -6955,18 +6952,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="382" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>7</v>
       </c>
       <c r="B382">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C382" s="5">
         <v>44013</v>
       </c>
       <c r="D382" s="5">
-        <v>44135</v>
+        <v>44104</v>
       </c>
       <c r="E382" t="s">
         <v>6</v>
@@ -6977,7 +6974,7 @@
         <v>7</v>
       </c>
       <c r="B383">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C383" s="5">
         <v>44013</v>
@@ -6991,16 +6988,16 @@
     </row>
     <row r="384" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B384">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C384" s="5">
-        <v>44028</v>
+        <v>44013</v>
       </c>
       <c r="D384" s="5">
-        <v>44104</v>
+        <v>44135</v>
       </c>
       <c r="E384" t="s">
         <v>6</v>
@@ -7011,13 +7008,13 @@
         <v>5</v>
       </c>
       <c r="B385">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C385" s="5">
-        <v>44105</v>
+        <v>44028</v>
       </c>
       <c r="D385" s="5">
-        <v>44316</v>
+        <v>44104</v>
       </c>
       <c r="E385" t="s">
         <v>6</v>
@@ -7025,33 +7022,33 @@
     </row>
     <row r="386" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B386">
+        <v>13</v>
+      </c>
+      <c r="C386" s="5">
+        <v>44105</v>
+      </c>
+      <c r="D386" s="5">
+        <v>44316</v>
+      </c>
+      <c r="E386" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="387" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A387" t="s">
+        <v>7</v>
+      </c>
+      <c r="B387">
         <v>10</v>
       </c>
-      <c r="C386" s="5">
+      <c r="C387" s="5">
         <v>44197</v>
       </c>
-      <c r="D386" s="5">
+      <c r="D387" s="5">
         <v>44214</v>
-      </c>
-      <c r="E386" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="387" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A387" t="s">
-        <v>5</v>
-      </c>
-      <c r="B387">
-        <v>5</v>
-      </c>
-      <c r="C387" s="5">
-        <v>44256</v>
-      </c>
-      <c r="D387" s="5">
-        <v>44316</v>
       </c>
       <c r="E387" t="s">
         <v>6</v>
@@ -7062,13 +7059,13 @@
         <v>5</v>
       </c>
       <c r="B388">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C388" s="5">
-        <v>44317</v>
+        <v>44256</v>
       </c>
       <c r="D388" s="5">
-        <v>44469</v>
+        <v>44316</v>
       </c>
       <c r="E388" t="s">
         <v>6</v>
@@ -7076,16 +7073,16 @@
     </row>
     <row r="389" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B389">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C389" s="5">
-        <v>44363</v>
+        <v>44317</v>
       </c>
       <c r="D389" s="5">
-        <v>44500</v>
+        <v>44469</v>
       </c>
       <c r="E389" t="s">
         <v>6</v>
@@ -7096,13 +7093,13 @@
         <v>7</v>
       </c>
       <c r="B390">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C390" s="5">
         <v>44363</v>
       </c>
       <c r="D390" s="5">
-        <v>44469</v>
+        <v>44500</v>
       </c>
       <c r="E390" t="s">
         <v>6</v>
@@ -7110,13 +7107,13 @@
     </row>
     <row r="391" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B391">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C391" s="5">
-        <v>44378</v>
+        <v>44363</v>
       </c>
       <c r="D391" s="5">
         <v>44469</v>
@@ -7130,7 +7127,7 @@
         <v>5</v>
       </c>
       <c r="B392">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C392" s="5">
         <v>44378</v>
@@ -7147,13 +7144,13 @@
         <v>5</v>
       </c>
       <c r="B393">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C393" s="5">
         <v>44378</v>
       </c>
       <c r="D393" s="5">
-        <v>44384</v>
+        <v>44469</v>
       </c>
       <c r="E393" t="s">
         <v>6</v>
@@ -7161,16 +7158,16 @@
     </row>
     <row r="394" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B394">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C394" s="5">
         <v>44378</v>
       </c>
       <c r="D394" s="5">
-        <v>44469</v>
+        <v>44384</v>
       </c>
       <c r="E394" t="s">
         <v>6</v>
@@ -7178,13 +7175,13 @@
     </row>
     <row r="395" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B395">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C395" s="5">
-        <v>44393</v>
+        <v>44378</v>
       </c>
       <c r="D395" s="5">
         <v>44469</v>
@@ -7195,16 +7192,16 @@
     </row>
     <row r="396" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B396">
-        <v>81</v>
+        <v>9</v>
       </c>
       <c r="C396" s="5">
-        <v>44409</v>
+        <v>44393</v>
       </c>
       <c r="D396" s="5">
-        <v>44458</v>
+        <v>44469</v>
       </c>
       <c r="E396" t="s">
         <v>6</v>
@@ -7212,13 +7209,13 @@
     </row>
     <row r="397" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B397">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C397" s="5">
-        <v>44422</v>
+        <v>44409</v>
       </c>
       <c r="D397" s="5">
         <v>44458</v>
@@ -7227,18 +7224,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="398" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B398">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="C398" s="5">
-        <v>44470</v>
+        <v>44422</v>
       </c>
       <c r="D398" s="5">
-        <v>44500</v>
+        <v>44458</v>
+      </c>
+      <c r="E398" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="399" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -7246,50 +7246,47 @@
         <v>7</v>
       </c>
       <c r="B399">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C399" s="5">
         <v>44470</v>
       </c>
       <c r="D399" s="5">
-        <v>44530</v>
+        <v>44500</v>
       </c>
     </row>
     <row r="400" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B400">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C400" s="5">
         <v>44470</v>
       </c>
       <c r="D400" s="5">
-        <v>44681</v>
-      </c>
-      <c r="E400" t="s">
-        <v>6</v>
+        <v>44530</v>
       </c>
     </row>
     <row r="401" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B401">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C401" s="5">
-        <v>44562</v>
+        <v>44470</v>
       </c>
       <c r="D401" s="5">
-        <v>44563</v>
+        <v>44681</v>
       </c>
       <c r="E401" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="402" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>7</v>
       </c>
@@ -7297,16 +7294,16 @@
         <v>10</v>
       </c>
       <c r="C402" s="5">
-        <v>44564</v>
+        <v>44562</v>
       </c>
       <c r="D402" s="5">
-        <v>44564</v>
+        <v>44563</v>
       </c>
       <c r="E402" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="403" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>7</v>
       </c>
@@ -7314,16 +7311,16 @@
         <v>10</v>
       </c>
       <c r="C403" s="5">
-        <v>44569</v>
+        <v>44564</v>
       </c>
       <c r="D403" s="5">
-        <v>44569</v>
+        <v>44564</v>
       </c>
       <c r="E403" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="404" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>7</v>
       </c>
@@ -7331,16 +7328,16 @@
         <v>10</v>
       </c>
       <c r="C404" s="5">
-        <v>44570</v>
+        <v>44569</v>
       </c>
       <c r="D404" s="5">
-        <v>44570</v>
+        <v>44569</v>
       </c>
       <c r="E404" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="405" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>7</v>
       </c>
@@ -7348,16 +7345,16 @@
         <v>10</v>
       </c>
       <c r="C405" s="5">
-        <v>44571</v>
+        <v>44570</v>
       </c>
       <c r="D405" s="5">
-        <v>44571</v>
+        <v>44570</v>
       </c>
       <c r="E405" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="406" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>7</v>
       </c>
@@ -7365,16 +7362,16 @@
         <v>10</v>
       </c>
       <c r="C406" s="5">
-        <v>44616</v>
+        <v>44571</v>
       </c>
       <c r="D406" s="5">
-        <v>44616</v>
+        <v>44571</v>
       </c>
       <c r="E406" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="407" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>7</v>
       </c>
@@ -7382,16 +7379,16 @@
         <v>10</v>
       </c>
       <c r="C407" s="5">
-        <v>44617</v>
+        <v>44616</v>
       </c>
       <c r="D407" s="5">
-        <v>44617</v>
+        <v>44616</v>
       </c>
       <c r="E407" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="408" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>7</v>
       </c>
@@ -7399,16 +7396,16 @@
         <v>10</v>
       </c>
       <c r="C408" s="5">
-        <v>44618</v>
+        <v>44617</v>
       </c>
       <c r="D408" s="5">
-        <v>44618</v>
+        <v>44617</v>
       </c>
       <c r="E408" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="409" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>7</v>
       </c>
@@ -7416,16 +7413,16 @@
         <v>10</v>
       </c>
       <c r="C409" s="5">
-        <v>44623</v>
+        <v>44618</v>
       </c>
       <c r="D409" s="5">
-        <v>44623</v>
+        <v>44618</v>
       </c>
       <c r="E409" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="410" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>7</v>
       </c>
@@ -7433,16 +7430,16 @@
         <v>10</v>
       </c>
       <c r="C410" s="5">
-        <v>44624</v>
+        <v>44623</v>
       </c>
       <c r="D410" s="5">
-        <v>44624</v>
+        <v>44623</v>
       </c>
       <c r="E410" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="411" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>7</v>
       </c>
@@ -7450,16 +7447,16 @@
         <v>10</v>
       </c>
       <c r="C411" s="5">
-        <v>44625</v>
+        <v>44624</v>
       </c>
       <c r="D411" s="5">
-        <v>44625</v>
+        <v>44624</v>
       </c>
       <c r="E411" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="412" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>7</v>
       </c>
@@ -7467,16 +7464,16 @@
         <v>10</v>
       </c>
       <c r="C412" s="5">
-        <v>44630</v>
+        <v>44625</v>
       </c>
       <c r="D412" s="5">
-        <v>44630</v>
+        <v>44625</v>
       </c>
       <c r="E412" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="413" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>7</v>
       </c>
@@ -7484,16 +7481,16 @@
         <v>10</v>
       </c>
       <c r="C413" s="5">
-        <v>44631</v>
+        <v>44630</v>
       </c>
       <c r="D413" s="5">
-        <v>44631</v>
+        <v>44630</v>
       </c>
       <c r="E413" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="414" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>7</v>
       </c>
@@ -7501,16 +7498,16 @@
         <v>10</v>
       </c>
       <c r="C414" s="5">
-        <v>44632</v>
+        <v>44631</v>
       </c>
       <c r="D414" s="5">
-        <v>44632</v>
+        <v>44631</v>
       </c>
       <c r="E414" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="415" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>7</v>
       </c>
@@ -7518,16 +7515,16 @@
         <v>10</v>
       </c>
       <c r="C415" s="5">
-        <v>44636</v>
+        <v>44632</v>
       </c>
       <c r="D415" s="5">
-        <v>44637</v>
+        <v>44632</v>
       </c>
       <c r="E415" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="416" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>7</v>
       </c>
@@ -7535,16 +7532,16 @@
         <v>10</v>
       </c>
       <c r="C416" s="5">
-        <v>44638</v>
+        <v>44636</v>
       </c>
       <c r="D416" s="5">
-        <v>44638</v>
+        <v>44637</v>
       </c>
       <c r="E416" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="417" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>7</v>
       </c>
@@ -7552,16 +7549,16 @@
         <v>10</v>
       </c>
       <c r="C417" s="5">
-        <v>44639</v>
+        <v>44638</v>
       </c>
       <c r="D417" s="5">
-        <v>44639</v>
+        <v>44638</v>
       </c>
       <c r="E417" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="418" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>7</v>
       </c>
@@ -7569,16 +7566,16 @@
         <v>10</v>
       </c>
       <c r="C418" s="5">
-        <v>44640</v>
+        <v>44639</v>
       </c>
       <c r="D418" s="5">
-        <v>44640</v>
+        <v>44639</v>
       </c>
       <c r="E418" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="419" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
         <v>7</v>
       </c>
@@ -7586,16 +7583,16 @@
         <v>10</v>
       </c>
       <c r="C419" s="5">
-        <v>44641</v>
+        <v>44640</v>
       </c>
       <c r="D419" s="5">
-        <v>44644</v>
+        <v>44640</v>
       </c>
       <c r="E419" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="420" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>7</v>
       </c>
@@ -7603,16 +7600,16 @@
         <v>10</v>
       </c>
       <c r="C420" s="5">
-        <v>44645</v>
+        <v>44641</v>
       </c>
       <c r="D420" s="5">
-        <v>44645</v>
+        <v>44644</v>
       </c>
       <c r="E420" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="421" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>7</v>
       </c>
@@ -7620,16 +7617,16 @@
         <v>10</v>
       </c>
       <c r="C421" s="5">
-        <v>44646</v>
+        <v>44645</v>
       </c>
       <c r="D421" s="5">
-        <v>44646</v>
+        <v>44645</v>
       </c>
       <c r="E421" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="422" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>7</v>
       </c>
@@ -7637,16 +7634,16 @@
         <v>10</v>
       </c>
       <c r="C422" s="5">
-        <v>44647</v>
+        <v>44646</v>
       </c>
       <c r="D422" s="5">
-        <v>44647</v>
+        <v>44646</v>
       </c>
       <c r="E422" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="423" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>7</v>
       </c>
@@ -7654,47 +7651,50 @@
         <v>10</v>
       </c>
       <c r="C423" s="5">
+        <v>44647</v>
+      </c>
+      <c r="D423" s="5">
+        <v>44647</v>
+      </c>
+      <c r="E423" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="424" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A424" t="s">
+        <v>7</v>
+      </c>
+      <c r="B424">
+        <v>10</v>
+      </c>
+      <c r="C424" s="5">
         <v>44648</v>
       </c>
-      <c r="D423" s="5">
+      <c r="D424" s="5">
         <v>44651</v>
       </c>
-      <c r="E423" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="424" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A424" t="s">
-        <v>5</v>
-      </c>
-      <c r="B424">
+      <c r="E424" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="425" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A425" t="s">
+        <v>5</v>
+      </c>
+      <c r="B425">
         <v>13</v>
       </c>
-      <c r="C424" s="5">
+      <c r="C425" s="5">
         <v>44700</v>
       </c>
-      <c r="D424" s="5">
+      <c r="D425" s="5">
         <v>44798</v>
       </c>
-      <c r="E424" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="425" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A425" t="s">
-        <v>7</v>
-      </c>
-      <c r="B425">
-        <v>11</v>
-      </c>
-      <c r="C425" s="5">
-        <v>44713</v>
-      </c>
-      <c r="D425" s="5">
-        <v>44714</v>
-      </c>
-    </row>
-    <row r="426" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E425" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="426" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>7</v>
       </c>
@@ -7702,10 +7702,10 @@
         <v>11</v>
       </c>
       <c r="C426" s="5">
-        <v>44715</v>
+        <v>44713</v>
       </c>
       <c r="D426" s="5">
-        <v>44715</v>
+        <v>44714</v>
       </c>
     </row>
     <row r="427" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -7713,30 +7713,27 @@
         <v>7</v>
       </c>
       <c r="B427">
+        <v>11</v>
+      </c>
+      <c r="C427" s="5">
+        <v>44715</v>
+      </c>
+      <c r="D427" s="5">
+        <v>44715</v>
+      </c>
+    </row>
+    <row r="428" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A428" t="s">
+        <v>7</v>
+      </c>
+      <c r="B428">
         <v>10</v>
       </c>
-      <c r="C427" s="5">
+      <c r="C428" s="5">
         <v>44728</v>
       </c>
-      <c r="D427" s="5">
+      <c r="D428" s="5">
         <v>44865</v>
-      </c>
-      <c r="E427" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="428" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A428" t="s">
-        <v>5</v>
-      </c>
-      <c r="B428">
-        <v>5</v>
-      </c>
-      <c r="C428" s="5">
-        <v>44743</v>
-      </c>
-      <c r="D428" s="5">
-        <v>44746</v>
       </c>
       <c r="E428" t="s">
         <v>6</v>
@@ -7747,30 +7744,33 @@
         <v>5</v>
       </c>
       <c r="B429">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C429" s="5">
         <v>44743</v>
       </c>
       <c r="D429" s="5">
-        <v>44765</v>
+        <v>44746</v>
       </c>
       <c r="E429" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="430" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B430">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C430" s="5">
         <v>44743</v>
       </c>
       <c r="D430" s="5">
-        <v>44743</v>
+        <v>44765</v>
+      </c>
+      <c r="E430" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="431" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -7778,93 +7778,93 @@
         <v>7</v>
       </c>
       <c r="B431">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C431" s="5">
         <v>44743</v>
       </c>
       <c r="D431" s="5">
+        <v>44743</v>
+      </c>
+    </row>
+    <row r="432" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A432" t="s">
+        <v>7</v>
+      </c>
+      <c r="B432">
+        <v>12</v>
+      </c>
+      <c r="C432" s="5">
+        <v>44743</v>
+      </c>
+      <c r="D432" s="5">
         <v>44834</v>
-      </c>
-    </row>
-    <row r="432" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A432" t="s">
-        <v>7</v>
-      </c>
-      <c r="B432">
-        <v>11</v>
-      </c>
-      <c r="C432" s="5">
-        <v>44744</v>
-      </c>
-      <c r="D432" s="5">
-        <v>44744</v>
       </c>
     </row>
     <row r="433" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B433">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C433" s="5">
-        <v>44748</v>
+        <v>44744</v>
       </c>
       <c r="D433" s="5">
-        <v>44748</v>
-      </c>
-      <c r="E433" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="434" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44744</v>
+      </c>
+    </row>
+    <row r="434" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B434">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C434" s="5">
         <v>44748</v>
       </c>
       <c r="D434" s="5">
-        <v>44749</v>
+        <v>44748</v>
+      </c>
+      <c r="E434" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="435" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B435">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C435" s="5">
-        <v>44750</v>
+        <v>44748</v>
       </c>
       <c r="D435" s="5">
-        <f>C435</f>
-        <v>44750</v>
-      </c>
-      <c r="E435" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="436" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44749</v>
+      </c>
+    </row>
+    <row r="436" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B436">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C436" s="5">
         <v>44750</v>
       </c>
       <c r="D436" s="5">
+        <f>C436</f>
         <v>44750</v>
       </c>
-    </row>
-    <row r="437" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E436" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="437" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
         <v>7</v>
       </c>
@@ -7872,28 +7872,24 @@
         <v>11</v>
       </c>
       <c r="C437" s="5">
-        <v>44751</v>
+        <v>44750</v>
       </c>
       <c r="D437" s="5">
-        <v>44751</v>
+        <v>44750</v>
       </c>
     </row>
     <row r="438" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B438">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C438" s="5">
-        <v>44752</v>
+        <v>44751</v>
       </c>
       <c r="D438" s="5">
-        <f>C438</f>
-        <v>44752</v>
-      </c>
-      <c r="E438" t="s">
-        <v>6</v>
+        <v>44751</v>
       </c>
     </row>
     <row r="439" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -7904,11 +7900,11 @@
         <v>5</v>
       </c>
       <c r="C439" s="5">
-        <v>44754</v>
+        <v>44752</v>
       </c>
       <c r="D439" s="5">
         <f>C439</f>
-        <v>44754</v>
+        <v>44752</v>
       </c>
       <c r="E439" t="s">
         <v>6</v>
@@ -7922,11 +7918,11 @@
         <v>5</v>
       </c>
       <c r="C440" s="5">
-        <v>44756</v>
+        <v>44754</v>
       </c>
       <c r="D440" s="5">
         <f>C440</f>
-        <v>44756</v>
+        <v>44754</v>
       </c>
       <c r="E440" t="s">
         <v>6</v>
@@ -7937,13 +7933,14 @@
         <v>5</v>
       </c>
       <c r="B441">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C441" s="5">
         <v>44756</v>
       </c>
       <c r="D441" s="5">
-        <v>44758</v>
+        <f>C441</f>
+        <v>44756</v>
       </c>
       <c r="E441" t="s">
         <v>6</v>
@@ -7954,7 +7951,7 @@
         <v>5</v>
       </c>
       <c r="B442">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C442" s="5">
         <v>44756</v>
@@ -7971,13 +7968,12 @@
         <v>5</v>
       </c>
       <c r="B443">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C443" s="5">
-        <v>44758</v>
+        <v>44756</v>
       </c>
       <c r="D443" s="5">
-        <f>C443</f>
         <v>44758</v>
       </c>
       <c r="E443" t="s">
@@ -7992,11 +7988,11 @@
         <v>5</v>
       </c>
       <c r="C444" s="5">
-        <v>44760</v>
+        <v>44758</v>
       </c>
       <c r="D444" s="5">
         <f>C444</f>
-        <v>44760</v>
+        <v>44758</v>
       </c>
       <c r="E444" t="s">
         <v>6</v>
@@ -8010,11 +8006,11 @@
         <v>5</v>
       </c>
       <c r="C445" s="5">
-        <v>44762</v>
+        <v>44760</v>
       </c>
       <c r="D445" s="5">
         <f>C445</f>
-        <v>44762</v>
+        <v>44760</v>
       </c>
       <c r="E445" t="s">
         <v>6</v>
@@ -8025,13 +8021,14 @@
         <v>5</v>
       </c>
       <c r="B446">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C446" s="5">
-        <v>44763</v>
+        <v>44762</v>
       </c>
       <c r="D446" s="5">
-        <v>44765</v>
+        <f>C446</f>
+        <v>44762</v>
       </c>
       <c r="E446" t="s">
         <v>6</v>
@@ -8042,7 +8039,7 @@
         <v>5</v>
       </c>
       <c r="B447">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C447" s="5">
         <v>44763</v>
@@ -8059,14 +8056,13 @@
         <v>5</v>
       </c>
       <c r="B448">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C448" s="5">
-        <v>44764</v>
+        <v>44763</v>
       </c>
       <c r="D448" s="5">
-        <f>C448</f>
-        <v>44764</v>
+        <v>44765</v>
       </c>
       <c r="E448" t="s">
         <v>6</v>
@@ -8080,10 +8076,11 @@
         <v>5</v>
       </c>
       <c r="C449" s="5">
-        <v>44766</v>
+        <v>44764</v>
       </c>
       <c r="D449" s="5">
-        <v>44832</v>
+        <f>C449</f>
+        <v>44764</v>
       </c>
       <c r="E449" t="s">
         <v>6</v>
@@ -8094,10 +8091,10 @@
         <v>5</v>
       </c>
       <c r="B450">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C450" s="5">
-        <v>44769</v>
+        <v>44766</v>
       </c>
       <c r="D450" s="5">
         <v>44832</v>
@@ -8111,13 +8108,13 @@
         <v>5</v>
       </c>
       <c r="B451">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C451" s="5">
-        <v>44770</v>
+        <v>44769</v>
       </c>
       <c r="D451" s="5">
-        <v>44772</v>
+        <v>44832</v>
       </c>
       <c r="E451" t="s">
         <v>6</v>
@@ -8128,13 +8125,13 @@
         <v>5</v>
       </c>
       <c r="B452">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C452" s="5">
         <v>44770</v>
       </c>
       <c r="D452" s="5">
-        <v>44829</v>
+        <v>44772</v>
       </c>
       <c r="E452" t="s">
         <v>6</v>
@@ -8142,33 +8139,36 @@
     </row>
     <row r="453" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B453">
+        <v>9</v>
+      </c>
+      <c r="C453" s="5">
+        <v>44770</v>
+      </c>
+      <c r="D453" s="5">
+        <v>44829</v>
+      </c>
+      <c r="E453" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="454" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A454" t="s">
+        <v>7</v>
+      </c>
+      <c r="B454">
         <v>81</v>
       </c>
-      <c r="C453" s="5">
+      <c r="C454" s="5">
         <v>44774</v>
       </c>
-      <c r="D453" s="5">
+      <c r="D454" s="5">
         <v>44834</v>
       </c>
     </row>
-    <row r="454" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A454" t="s">
-        <v>7</v>
-      </c>
-      <c r="B454">
-        <v>11</v>
-      </c>
-      <c r="C454" s="5">
-        <v>44776</v>
-      </c>
-      <c r="D454" s="5">
-        <v>44777</v>
-      </c>
-    </row>
-    <row r="455" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
         <v>7</v>
       </c>
@@ -8176,13 +8176,13 @@
         <v>11</v>
       </c>
       <c r="C455" s="5">
-        <v>44778</v>
+        <v>44776</v>
       </c>
       <c r="D455" s="5">
-        <v>44778</v>
-      </c>
-    </row>
-    <row r="456" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44777</v>
+      </c>
+    </row>
+    <row r="456" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
         <v>7</v>
       </c>
@@ -8190,13 +8190,13 @@
         <v>11</v>
       </c>
       <c r="C456" s="5">
-        <v>44779</v>
+        <v>44778</v>
       </c>
       <c r="D456" s="5">
-        <v>44779</v>
-      </c>
-    </row>
-    <row r="457" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44778</v>
+      </c>
+    </row>
+    <row r="457" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
         <v>7</v>
       </c>
@@ -8204,13 +8204,13 @@
         <v>11</v>
       </c>
       <c r="C457" s="5">
-        <v>44783</v>
+        <v>44779</v>
       </c>
       <c r="D457" s="5">
-        <v>44784</v>
-      </c>
-    </row>
-    <row r="458" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44779</v>
+      </c>
+    </row>
+    <row r="458" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
         <v>7</v>
       </c>
@@ -8218,13 +8218,13 @@
         <v>11</v>
       </c>
       <c r="C458" s="5">
-        <v>44785</v>
+        <v>44783</v>
       </c>
       <c r="D458" s="5">
-        <v>44785</v>
-      </c>
-    </row>
-    <row r="459" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44784</v>
+      </c>
+    </row>
+    <row r="459" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
         <v>7</v>
       </c>
@@ -8232,24 +8232,24 @@
         <v>11</v>
       </c>
       <c r="C459" s="5">
-        <v>44786</v>
+        <v>44785</v>
       </c>
       <c r="D459" s="5">
-        <v>44786</v>
+        <v>44785</v>
       </c>
     </row>
     <row r="460" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B460">
-        <v>82</v>
+        <v>11</v>
       </c>
       <c r="C460" s="5">
         <v>44786</v>
       </c>
       <c r="D460" s="5">
-        <v>44823</v>
+        <v>44786</v>
       </c>
     </row>
     <row r="461" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8257,33 +8257,33 @@
         <v>5</v>
       </c>
       <c r="B461">
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="C461" s="5">
+        <v>44786</v>
+      </c>
+      <c r="D461" s="5">
+        <v>44823</v>
+      </c>
+    </row>
+    <row r="462" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A462" t="s">
+        <v>5</v>
+      </c>
+      <c r="B462">
+        <v>7</v>
+      </c>
+      <c r="C462" s="5">
         <v>44789</v>
       </c>
-      <c r="D461" s="5">
+      <c r="D462" s="5">
         <v>44834</v>
       </c>
-      <c r="E461" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="462" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A462" t="s">
-        <v>7</v>
-      </c>
-      <c r="B462">
-        <v>11</v>
-      </c>
-      <c r="C462" s="5">
-        <v>44790</v>
-      </c>
-      <c r="D462" s="5">
-        <v>44791</v>
-      </c>
-    </row>
-    <row r="463" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E462" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="463" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
         <v>7</v>
       </c>
@@ -8291,13 +8291,13 @@
         <v>11</v>
       </c>
       <c r="C463" s="5">
-        <v>44792</v>
+        <v>44790</v>
       </c>
       <c r="D463" s="5">
-        <v>44792</v>
-      </c>
-    </row>
-    <row r="464" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44791</v>
+      </c>
+    </row>
+    <row r="464" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
         <v>7</v>
       </c>
@@ -8305,13 +8305,13 @@
         <v>11</v>
       </c>
       <c r="C464" s="5">
-        <v>44793</v>
+        <v>44792</v>
       </c>
       <c r="D464" s="5">
-        <v>44793</v>
-      </c>
-    </row>
-    <row r="465" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44792</v>
+      </c>
+    </row>
+    <row r="465" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
         <v>7</v>
       </c>
@@ -8319,13 +8319,13 @@
         <v>11</v>
       </c>
       <c r="C465" s="5">
-        <v>44794</v>
+        <v>44793</v>
       </c>
       <c r="D465" s="5">
-        <v>44794</v>
-      </c>
-    </row>
-    <row r="466" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44793</v>
+      </c>
+    </row>
+    <row r="466" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
         <v>7</v>
       </c>
@@ -8333,13 +8333,13 @@
         <v>11</v>
       </c>
       <c r="C466" s="5">
-        <v>44795</v>
+        <v>44794</v>
       </c>
       <c r="D466" s="5">
-        <v>44798</v>
-      </c>
-    </row>
-    <row r="467" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44794</v>
+      </c>
+    </row>
+    <row r="467" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
         <v>7</v>
       </c>
@@ -8347,13 +8347,13 @@
         <v>11</v>
       </c>
       <c r="C467" s="5">
-        <v>44799</v>
+        <v>44795</v>
       </c>
       <c r="D467" s="5">
-        <v>44799</v>
-      </c>
-    </row>
-    <row r="468" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44798</v>
+      </c>
+    </row>
+    <row r="468" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
         <v>7</v>
       </c>
@@ -8361,13 +8361,13 @@
         <v>11</v>
       </c>
       <c r="C468" s="5">
-        <v>44800</v>
+        <v>44799</v>
       </c>
       <c r="D468" s="5">
-        <v>44800</v>
-      </c>
-    </row>
-    <row r="469" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44799</v>
+      </c>
+    </row>
+    <row r="469" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
         <v>7</v>
       </c>
@@ -8375,13 +8375,13 @@
         <v>11</v>
       </c>
       <c r="C469" s="5">
-        <v>44801</v>
+        <v>44800</v>
       </c>
       <c r="D469" s="5">
-        <v>44801</v>
-      </c>
-    </row>
-    <row r="470" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44800</v>
+      </c>
+    </row>
+    <row r="470" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
         <v>7</v>
       </c>
@@ -8389,44 +8389,44 @@
         <v>11</v>
       </c>
       <c r="C470" s="5">
-        <v>44802</v>
+        <v>44801</v>
       </c>
       <c r="D470" s="5">
-        <v>44805</v>
+        <v>44801</v>
       </c>
     </row>
     <row r="471" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B471">
+        <v>11</v>
+      </c>
+      <c r="C471" s="5">
+        <v>44802</v>
+      </c>
+      <c r="D471" s="5">
+        <v>44805</v>
+      </c>
+    </row>
+    <row r="472" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A472" t="s">
+        <v>5</v>
+      </c>
+      <c r="B472">
         <v>13</v>
       </c>
-      <c r="C471" s="5">
+      <c r="C472" s="5">
         <v>44804</v>
       </c>
-      <c r="D471" s="5">
+      <c r="D472" s="5">
         <v>44834</v>
       </c>
-      <c r="E471" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="472" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A472" t="s">
-        <v>7</v>
-      </c>
-      <c r="B472">
-        <v>11</v>
-      </c>
-      <c r="C472" s="5">
-        <v>44806</v>
-      </c>
-      <c r="D472" s="5">
-        <v>44806</v>
-      </c>
-    </row>
-    <row r="473" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E472" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="473" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
         <v>7</v>
       </c>
@@ -8434,13 +8434,13 @@
         <v>11</v>
       </c>
       <c r="C473" s="5">
-        <v>44807</v>
+        <v>44806</v>
       </c>
       <c r="D473" s="5">
-        <v>44807</v>
-      </c>
-    </row>
-    <row r="474" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44806</v>
+      </c>
+    </row>
+    <row r="474" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
         <v>7</v>
       </c>
@@ -8448,13 +8448,13 @@
         <v>11</v>
       </c>
       <c r="C474" s="5">
-        <v>44808</v>
+        <v>44807</v>
       </c>
       <c r="D474" s="5">
-        <v>44809</v>
-      </c>
-    </row>
-    <row r="475" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44807</v>
+      </c>
+    </row>
+    <row r="475" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A475" t="s">
         <v>7</v>
       </c>
@@ -8462,13 +8462,13 @@
         <v>11</v>
       </c>
       <c r="C475" s="5">
-        <v>44810</v>
+        <v>44808</v>
       </c>
       <c r="D475" s="5">
-        <v>44812</v>
-      </c>
-    </row>
-    <row r="476" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44809</v>
+      </c>
+    </row>
+    <row r="476" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
         <v>7</v>
       </c>
@@ -8476,13 +8476,13 @@
         <v>11</v>
       </c>
       <c r="C476" s="5">
-        <v>44813</v>
+        <v>44810</v>
       </c>
       <c r="D476" s="5">
-        <v>44813</v>
-      </c>
-    </row>
-    <row r="477" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44812</v>
+      </c>
+    </row>
+    <row r="477" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
         <v>7</v>
       </c>
@@ -8490,13 +8490,13 @@
         <v>11</v>
       </c>
       <c r="C477" s="5">
-        <v>44814</v>
+        <v>44813</v>
       </c>
       <c r="D477" s="5">
-        <v>44814</v>
-      </c>
-    </row>
-    <row r="478" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44813</v>
+      </c>
+    </row>
+    <row r="478" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
         <v>7</v>
       </c>
@@ -8504,13 +8504,13 @@
         <v>11</v>
       </c>
       <c r="C478" s="5">
-        <v>44815</v>
+        <v>44814</v>
       </c>
       <c r="D478" s="5">
-        <v>44815</v>
-      </c>
-    </row>
-    <row r="479" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44814</v>
+      </c>
+    </row>
+    <row r="479" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A479" t="s">
         <v>7</v>
       </c>
@@ -8518,13 +8518,13 @@
         <v>11</v>
       </c>
       <c r="C479" s="5">
-        <v>44816</v>
+        <v>44815</v>
       </c>
       <c r="D479" s="5">
-        <v>44819</v>
-      </c>
-    </row>
-    <row r="480" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44815</v>
+      </c>
+    </row>
+    <row r="480" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
         <v>7</v>
       </c>
@@ -8532,13 +8532,13 @@
         <v>11</v>
       </c>
       <c r="C480" s="5">
-        <v>44820</v>
+        <v>44816</v>
       </c>
       <c r="D480" s="5">
-        <v>44820</v>
-      </c>
-    </row>
-    <row r="481" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44819</v>
+      </c>
+    </row>
+    <row r="481" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
         <v>7</v>
       </c>
@@ -8546,13 +8546,13 @@
         <v>11</v>
       </c>
       <c r="C481" s="5">
-        <v>44821</v>
+        <v>44820</v>
       </c>
       <c r="D481" s="5">
-        <v>44821</v>
-      </c>
-    </row>
-    <row r="482" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44820</v>
+      </c>
+    </row>
+    <row r="482" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
         <v>7</v>
       </c>
@@ -8560,13 +8560,13 @@
         <v>11</v>
       </c>
       <c r="C482" s="5">
-        <v>44822</v>
+        <v>44821</v>
       </c>
       <c r="D482" s="5">
-        <v>44822</v>
-      </c>
-    </row>
-    <row r="483" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44821</v>
+      </c>
+    </row>
+    <row r="483" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
         <v>7</v>
       </c>
@@ -8574,13 +8574,13 @@
         <v>11</v>
       </c>
       <c r="C483" s="5">
-        <v>44823</v>
+        <v>44822</v>
       </c>
       <c r="D483" s="5">
-        <v>44826</v>
-      </c>
-    </row>
-    <row r="484" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44822</v>
+      </c>
+    </row>
+    <row r="484" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
         <v>7</v>
       </c>
@@ -8588,13 +8588,13 @@
         <v>11</v>
       </c>
       <c r="C484" s="5">
-        <v>44827</v>
+        <v>44823</v>
       </c>
       <c r="D484" s="5">
-        <v>44827</v>
-      </c>
-    </row>
-    <row r="485" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44826</v>
+      </c>
+    </row>
+    <row r="485" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
         <v>7</v>
       </c>
@@ -8602,13 +8602,13 @@
         <v>11</v>
       </c>
       <c r="C485" s="5">
-        <v>44828</v>
+        <v>44827</v>
       </c>
       <c r="D485" s="5">
-        <v>44828</v>
-      </c>
-    </row>
-    <row r="486" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44827</v>
+      </c>
+    </row>
+    <row r="486" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
         <v>7</v>
       </c>
@@ -8616,13 +8616,13 @@
         <v>11</v>
       </c>
       <c r="C486" s="5">
-        <v>44829</v>
+        <v>44828</v>
       </c>
       <c r="D486" s="5">
-        <v>44829</v>
-      </c>
-    </row>
-    <row r="487" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44828</v>
+      </c>
+    </row>
+    <row r="487" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
         <v>7</v>
       </c>
@@ -8630,13 +8630,13 @@
         <v>11</v>
       </c>
       <c r="C487" s="5">
-        <v>44830</v>
+        <v>44829</v>
       </c>
       <c r="D487" s="5">
-        <v>44833</v>
-      </c>
-    </row>
-    <row r="488" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44829</v>
+      </c>
+    </row>
+    <row r="488" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
         <v>7</v>
       </c>
@@ -8644,13 +8644,13 @@
         <v>11</v>
       </c>
       <c r="C488" s="5">
-        <v>44834</v>
+        <v>44830</v>
       </c>
       <c r="D488" s="5">
-        <v>44834</v>
-      </c>
-    </row>
-    <row r="489" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44833</v>
+      </c>
+    </row>
+    <row r="489" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
         <v>7</v>
       </c>
@@ -8658,10 +8658,10 @@
         <v>11</v>
       </c>
       <c r="C489" s="5">
-        <v>44835</v>
+        <v>44834</v>
       </c>
       <c r="D489" s="5">
-        <v>44865</v>
+        <v>44834</v>
       </c>
     </row>
     <row r="490" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8669,7 +8669,7 @@
         <v>7</v>
       </c>
       <c r="B490">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C490" s="5">
         <v>44835</v>
@@ -8680,48 +8680,62 @@
     </row>
     <row r="491" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B491">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C491" s="5">
         <v>44835</v>
       </c>
       <c r="D491" s="5">
-        <v>45046</v>
-      </c>
-      <c r="E491" t="s">
-        <v>6</v>
+        <v>44865</v>
       </c>
     </row>
     <row r="492" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B492">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="C492" s="5">
         <v>44835</v>
       </c>
       <c r="D492" s="5">
+        <v>45046</v>
+      </c>
+      <c r="E492" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="493" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A493" t="s">
+        <v>7</v>
+      </c>
+      <c r="B493">
+        <v>81</v>
+      </c>
+      <c r="C493" s="5">
+        <v>44835</v>
+      </c>
+      <c r="D493" s="5">
         <v>44843</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E492" xr:uid="{9536AF9F-EFE7-469A-8B3B-7525E4B6BE61}">
+  <autoFilter ref="A1:E493" xr:uid="{9536AF9F-EFE7-469A-8B3B-7525E4B6BE61}">
     <filterColumn colId="1">
       <filters>
-        <filter val="11"/>
+        <filter val="10"/>
       </filters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:E449">
-      <sortCondition ref="C264:C492"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:E450">
+      <sortCondition ref="C264:C493"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E492">
-    <sortCondition ref="C207:C492"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E493">
+    <sortCondition ref="C207:C493"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix to area 7 2017 (it was closed not open)
</commit_message>
<xml_diff>
--- a/data/sources/coho_regulations.xlsx
+++ b/data/sources/coho_regulations.xlsx
@@ -5,18 +5,18 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/tyler_garber_dfw_wa_gov/Documents/sport_harvest/sport/sport_harvest_estimator/data/sources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\sport_harvest\sport\sport_harvest_estimator\data\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{3F960066-A2E8-41E3-8CB8-A4E7D7F70CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDE6AF75-02D0-4D23-BAA2-3895173C3981}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2489E3-9C7E-4806-A1CE-55F0E427468C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29325" yWindow="4005" windowWidth="19185" windowHeight="10185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8355" yWindow="825" windowWidth="19185" windowHeight="10185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="coho_regulations" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">coho_regulations!$A$1:$E$493</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">coho_regulations!$A$1:$E$492</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="8">
   <si>
     <t>regulation_type_code</t>
   </si>
@@ -471,11 +471,11 @@
   <sheetPr codeName="Sheet1" filterMode="1">
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:E493"/>
+  <dimension ref="A1:E492"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A250" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C271" sqref="C271"/>
+      <pane ySplit="1" topLeftCell="A204" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D335" sqref="D335"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,7 +572,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -589,7 +589,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -657,7 +657,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -708,7 +708,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -776,7 +776,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -793,7 +793,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -997,7 +997,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>7</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>7</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>7</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>5</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>7</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>7</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>7</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>7</v>
       </c>
@@ -1830,7 +1830,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>7</v>
       </c>
@@ -1898,7 +1898,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>5</v>
       </c>
@@ -1966,7 +1966,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>7</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>7</v>
       </c>
@@ -2204,7 +2204,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="102" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>7</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>7</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="107" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>5</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="112" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>7</v>
       </c>
@@ -2476,7 +2476,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="118" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>7</v>
       </c>
@@ -2646,7 +2646,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="128" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>7</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>7</v>
       </c>
@@ -2731,7 +2731,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="133" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>5</v>
       </c>
@@ -2833,7 +2833,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="139" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>7</v>
       </c>
@@ -2935,7 +2935,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="145" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>7</v>
       </c>
@@ -3105,7 +3105,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="155" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>7</v>
       </c>
@@ -3122,7 +3122,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>7</v>
       </c>
@@ -3190,7 +3190,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="160" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>5</v>
       </c>
@@ -3326,7 +3326,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="168" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>7</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="179" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>7</v>
       </c>
@@ -3530,7 +3530,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>7</v>
       </c>
@@ -3598,7 +3598,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="184" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>5</v>
       </c>
@@ -3683,7 +3683,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="189" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>7</v>
       </c>
@@ -3768,7 +3768,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="194" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>7</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="204" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>7</v>
       </c>
@@ -3955,7 +3955,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>7</v>
       </c>
@@ -4023,7 +4023,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="209" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>5</v>
       </c>
@@ -4142,7 +4142,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="216" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>7</v>
       </c>
@@ -4312,7 +4312,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="226" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>7</v>
       </c>
@@ -4346,7 +4346,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>7</v>
       </c>
@@ -4397,7 +4397,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="231" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>5</v>
       </c>
@@ -4482,7 +4482,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="236" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>7</v>
       </c>
@@ -4533,7 +4533,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="239" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>7</v>
       </c>
@@ -4686,7 +4686,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="248" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>7</v>
       </c>
@@ -4720,7 +4720,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>7</v>
       </c>
@@ -4771,7 +4771,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="253" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>5</v>
       </c>
@@ -4890,7 +4890,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="260" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>7</v>
       </c>
@@ -5043,7 +5043,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="269" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>7</v>
       </c>
@@ -5077,7 +5077,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>7</v>
       </c>
@@ -5128,7 +5128,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="274" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>5</v>
       </c>
@@ -5264,7 +5264,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="282" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>7</v>
       </c>
@@ -5417,7 +5417,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>7</v>
       </c>
@@ -5468,7 +5468,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="294" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>5</v>
       </c>
@@ -5629,7 +5629,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="304" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>7</v>
       </c>
@@ -5714,7 +5714,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="309" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>7</v>
       </c>
@@ -5731,7 +5731,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>7</v>
       </c>
@@ -5971,13 +5971,13 @@
         <v>7</v>
       </c>
       <c r="B324">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C324" s="5">
         <v>42917</v>
       </c>
       <c r="D324" s="5">
-        <v>43008</v>
+        <v>43069</v>
       </c>
       <c r="E324" t="s">
         <v>6</v>
@@ -5985,16 +5985,16 @@
     </row>
     <row r="325" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B325">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C325" s="5">
-        <v>42917</v>
+        <v>42932</v>
       </c>
       <c r="D325" s="5">
-        <v>43069</v>
+        <v>42982</v>
       </c>
       <c r="E325" t="s">
         <v>6</v>
@@ -6005,30 +6005,30 @@
         <v>5</v>
       </c>
       <c r="B326">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C326" s="5">
-        <v>42932</v>
+        <v>42917</v>
       </c>
       <c r="D326" s="5">
+        <v>43159</v>
+      </c>
+      <c r="E326" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="327" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
+        <v>5</v>
+      </c>
+      <c r="B327">
+        <v>82</v>
+      </c>
+      <c r="C327" s="5">
+        <v>42948</v>
+      </c>
+      <c r="D327" s="5">
         <v>42982</v>
-      </c>
-      <c r="E326" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A327" t="s">
-        <v>5</v>
-      </c>
-      <c r="B327">
-        <v>10</v>
-      </c>
-      <c r="C327" s="5">
-        <v>42917</v>
-      </c>
-      <c r="D327" s="5">
-        <v>43159</v>
       </c>
       <c r="E327" t="s">
         <v>6</v>
@@ -6039,13 +6039,13 @@
         <v>5</v>
       </c>
       <c r="B328">
-        <v>82</v>
+        <v>13</v>
       </c>
       <c r="C328" s="5">
-        <v>42948</v>
+        <v>43009</v>
       </c>
       <c r="D328" s="5">
-        <v>42982</v>
+        <v>43220</v>
       </c>
       <c r="E328" t="s">
         <v>6</v>
@@ -6056,10 +6056,10 @@
         <v>5</v>
       </c>
       <c r="B329">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C329" s="5">
-        <v>43009</v>
+        <v>43040</v>
       </c>
       <c r="D329" s="5">
         <v>43220</v>
@@ -6070,13 +6070,13 @@
     </row>
     <row r="330" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B330">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C330" s="5">
-        <v>43040</v>
+        <v>43070</v>
       </c>
       <c r="D330" s="5">
         <v>43220</v>
@@ -6087,16 +6087,16 @@
     </row>
     <row r="331" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B331">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C331" s="5">
-        <v>43070</v>
+        <v>43221</v>
       </c>
       <c r="D331" s="5">
-        <v>43220</v>
+        <v>43373</v>
       </c>
       <c r="E331" t="s">
         <v>6</v>
@@ -6104,16 +6104,16 @@
     </row>
     <row r="332" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B332">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C332" s="5">
-        <v>43221</v>
+        <v>43252</v>
       </c>
       <c r="D332" s="5">
-        <v>43373</v>
+        <v>43297</v>
       </c>
       <c r="E332" t="s">
         <v>6</v>
@@ -6121,16 +6121,16 @@
     </row>
     <row r="333" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B333">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C333" s="5">
-        <v>43252</v>
+        <v>43282</v>
       </c>
       <c r="D333" s="5">
-        <v>43297</v>
+        <v>43373</v>
       </c>
       <c r="E333" t="s">
         <v>6</v>
@@ -6141,7 +6141,7 @@
         <v>5</v>
       </c>
       <c r="B334">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C334" s="5">
         <v>43282</v>
@@ -6153,12 +6153,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="335" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B335">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C335" s="5">
         <v>43282</v>
@@ -6175,30 +6175,30 @@
         <v>7</v>
       </c>
       <c r="B336">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C336" s="5">
+        <v>43252</v>
+      </c>
+      <c r="D336" s="5">
+        <v>43419</v>
+      </c>
+      <c r="E336" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="337" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
+        <v>7</v>
+      </c>
+      <c r="B337">
+        <v>12</v>
+      </c>
+      <c r="C337" s="5">
         <v>43282</v>
       </c>
-      <c r="D336" s="5">
-        <v>43373</v>
-      </c>
-      <c r="E336" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A337" t="s">
-        <v>7</v>
-      </c>
-      <c r="B337">
-        <v>10</v>
-      </c>
-      <c r="C337" s="5">
-        <v>43252</v>
-      </c>
       <c r="D337" s="5">
-        <v>43419</v>
+        <v>43404</v>
       </c>
       <c r="E337" t="s">
         <v>6</v>
@@ -6206,16 +6206,16 @@
     </row>
     <row r="338" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B338">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C338" s="5">
-        <v>43282</v>
+        <v>43297</v>
       </c>
       <c r="D338" s="5">
-        <v>43404</v>
+        <v>43373</v>
       </c>
       <c r="E338" t="s">
         <v>6</v>
@@ -6223,16 +6223,16 @@
     </row>
     <row r="339" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B339">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C339" s="5">
-        <v>43297</v>
+        <v>43301</v>
       </c>
       <c r="D339" s="5">
-        <v>43373</v>
+        <v>43304</v>
       </c>
       <c r="E339" t="s">
         <v>6</v>
@@ -6246,10 +6246,10 @@
         <v>11</v>
       </c>
       <c r="C340" s="5">
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D340" s="5">
-        <v>43304</v>
+        <v>43311</v>
       </c>
       <c r="E340" t="s">
         <v>6</v>
@@ -6263,10 +6263,10 @@
         <v>11</v>
       </c>
       <c r="C341" s="5">
-        <v>43308</v>
+        <v>43312</v>
       </c>
       <c r="D341" s="5">
-        <v>43311</v>
+        <v>43373</v>
       </c>
       <c r="E341" t="s">
         <v>6</v>
@@ -6277,10 +6277,10 @@
         <v>7</v>
       </c>
       <c r="B342">
-        <v>11</v>
+        <v>81</v>
       </c>
       <c r="C342" s="5">
-        <v>43312</v>
+        <v>43313</v>
       </c>
       <c r="D342" s="5">
         <v>43373</v>
@@ -6294,13 +6294,13 @@
         <v>7</v>
       </c>
       <c r="B343">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C343" s="5">
         <v>43313</v>
       </c>
       <c r="D343" s="5">
-        <v>43373</v>
+        <v>43366</v>
       </c>
       <c r="E343" t="s">
         <v>6</v>
@@ -6308,16 +6308,16 @@
     </row>
     <row r="344" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B344">
-        <v>82</v>
+        <v>13</v>
       </c>
       <c r="C344" s="5">
-        <v>43313</v>
+        <v>43374</v>
       </c>
       <c r="D344" s="5">
-        <v>43366</v>
+        <v>43585</v>
       </c>
       <c r="E344" t="s">
         <v>6</v>
@@ -6325,13 +6325,13 @@
     </row>
     <row r="345" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B345">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C345" s="5">
-        <v>43374</v>
+        <v>43405</v>
       </c>
       <c r="D345" s="5">
         <v>43585</v>
@@ -6345,10 +6345,10 @@
         <v>7</v>
       </c>
       <c r="B346">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C346" s="5">
-        <v>43405</v>
+        <v>43374</v>
       </c>
       <c r="D346" s="5">
         <v>43585</v>
@@ -6362,30 +6362,30 @@
         <v>7</v>
       </c>
       <c r="B347">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C347" s="5">
-        <v>43374</v>
+        <v>43466</v>
       </c>
       <c r="D347" s="5">
-        <v>43585</v>
+        <v>43555</v>
       </c>
       <c r="E347" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B348">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C348" s="5">
-        <v>43466</v>
+        <v>43497</v>
       </c>
       <c r="D348" s="5">
-        <v>43555</v>
+        <v>43570</v>
       </c>
       <c r="E348" t="s">
         <v>6</v>
@@ -6396,13 +6396,13 @@
         <v>5</v>
       </c>
       <c r="B349">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C349" s="5">
-        <v>43497</v>
+        <v>43512</v>
       </c>
       <c r="D349" s="5">
-        <v>43570</v>
+        <v>43585</v>
       </c>
       <c r="E349" t="s">
         <v>6</v>
@@ -6413,13 +6413,13 @@
         <v>5</v>
       </c>
       <c r="B350">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C350" s="5">
-        <v>43512</v>
+        <v>43586</v>
       </c>
       <c r="D350" s="5">
-        <v>43585</v>
+        <v>43738</v>
       </c>
       <c r="E350" t="s">
         <v>6</v>
@@ -6427,33 +6427,33 @@
     </row>
     <row r="351" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B351">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C351" s="5">
-        <v>43586</v>
+        <v>43617</v>
       </c>
       <c r="D351" s="5">
+        <v>43784</v>
+      </c>
+      <c r="E351" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="352" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
+        <v>5</v>
+      </c>
+      <c r="B352">
+        <v>5</v>
+      </c>
+      <c r="C352" s="5">
+        <v>43647</v>
+      </c>
+      <c r="D352" s="5">
         <v>43738</v>
-      </c>
-      <c r="E351" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A352" t="s">
-        <v>7</v>
-      </c>
-      <c r="B352">
-        <v>10</v>
-      </c>
-      <c r="C352" s="5">
-        <v>43617</v>
-      </c>
-      <c r="D352" s="5">
-        <v>43784</v>
       </c>
       <c r="E352" t="s">
         <v>6</v>
@@ -6464,7 +6464,7 @@
         <v>5</v>
       </c>
       <c r="B353">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C353" s="5">
         <v>43647</v>
@@ -6476,18 +6476,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="354" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B354">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C354" s="5">
         <v>43647</v>
       </c>
       <c r="D354" s="5">
-        <v>43738</v>
+        <v>43677</v>
       </c>
       <c r="E354" t="s">
         <v>6</v>
@@ -6498,13 +6498,13 @@
         <v>7</v>
       </c>
       <c r="B355">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C355" s="5">
         <v>43647</v>
       </c>
       <c r="D355" s="5">
-        <v>43677</v>
+        <v>43649</v>
       </c>
       <c r="E355" t="s">
         <v>6</v>
@@ -6515,13 +6515,13 @@
         <v>7</v>
       </c>
       <c r="B356">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C356" s="5">
         <v>43647</v>
       </c>
       <c r="D356" s="5">
-        <v>43649</v>
+        <v>43769</v>
       </c>
       <c r="E356" t="s">
         <v>6</v>
@@ -6532,13 +6532,13 @@
         <v>7</v>
       </c>
       <c r="B357">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C357" s="5">
-        <v>43647</v>
+        <v>43652</v>
       </c>
       <c r="D357" s="5">
-        <v>43769</v>
+        <v>43656</v>
       </c>
       <c r="E357" t="s">
         <v>6</v>
@@ -6552,10 +6552,10 @@
         <v>11</v>
       </c>
       <c r="C358" s="5">
-        <v>43652</v>
+        <v>43659</v>
       </c>
       <c r="D358" s="5">
-        <v>43656</v>
+        <v>43663</v>
       </c>
       <c r="E358" t="s">
         <v>6</v>
@@ -6569,10 +6569,10 @@
         <v>11</v>
       </c>
       <c r="C359" s="5">
-        <v>43659</v>
+        <v>43666</v>
       </c>
       <c r="D359" s="5">
-        <v>43663</v>
+        <v>43670</v>
       </c>
       <c r="E359" t="s">
         <v>6</v>
@@ -6580,16 +6580,16 @@
     </row>
     <row r="360" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B360">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C360" s="5">
-        <v>43666</v>
+        <v>43671</v>
       </c>
       <c r="D360" s="5">
-        <v>43670</v>
+        <v>43738</v>
       </c>
       <c r="E360" t="s">
         <v>6</v>
@@ -6597,16 +6597,16 @@
     </row>
     <row r="361" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B361">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C361" s="5">
-        <v>43671</v>
+        <v>43673</v>
       </c>
       <c r="D361" s="5">
-        <v>43738</v>
+        <v>43677</v>
       </c>
       <c r="E361" t="s">
         <v>6</v>
@@ -6617,13 +6617,13 @@
         <v>7</v>
       </c>
       <c r="B362">
-        <v>11</v>
+        <v>81</v>
       </c>
       <c r="C362" s="5">
-        <v>43673</v>
+        <v>43678</v>
       </c>
       <c r="D362" s="5">
-        <v>43677</v>
+        <v>43769</v>
       </c>
       <c r="E362" t="s">
         <v>6</v>
@@ -6634,13 +6634,13 @@
         <v>7</v>
       </c>
       <c r="B363">
-        <v>81</v>
+        <v>11</v>
       </c>
       <c r="C363" s="5">
-        <v>43678</v>
+        <v>43680</v>
       </c>
       <c r="D363" s="5">
-        <v>43769</v>
+        <v>43684</v>
       </c>
       <c r="E363" t="s">
         <v>6</v>
@@ -6654,10 +6654,10 @@
         <v>11</v>
       </c>
       <c r="C364" s="5">
-        <v>43680</v>
+        <v>43687</v>
       </c>
       <c r="D364" s="5">
-        <v>43684</v>
+        <v>43691</v>
       </c>
       <c r="E364" t="s">
         <v>6</v>
@@ -6665,16 +6665,16 @@
     </row>
     <row r="365" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B365">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="C365" s="5">
-        <v>43687</v>
+        <v>43693</v>
       </c>
       <c r="D365" s="5">
-        <v>43691</v>
+        <v>43723</v>
       </c>
       <c r="E365" t="s">
         <v>6</v>
@@ -6682,16 +6682,16 @@
     </row>
     <row r="366" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B366">
-        <v>82</v>
+        <v>11</v>
       </c>
       <c r="C366" s="5">
-        <v>43693</v>
+        <v>43694</v>
       </c>
       <c r="D366" s="5">
-        <v>43723</v>
+        <v>43698</v>
       </c>
       <c r="E366" t="s">
         <v>6</v>
@@ -6705,10 +6705,10 @@
         <v>11</v>
       </c>
       <c r="C367" s="5">
-        <v>43694</v>
+        <v>43701</v>
       </c>
       <c r="D367" s="5">
-        <v>43698</v>
+        <v>43702</v>
       </c>
       <c r="E367" t="s">
         <v>6</v>
@@ -6722,24 +6722,24 @@
         <v>11</v>
       </c>
       <c r="C368" s="5">
-        <v>43701</v>
+        <v>43703</v>
       </c>
       <c r="D368" s="5">
-        <v>43702</v>
+        <v>43738</v>
       </c>
       <c r="E368" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="369" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>7</v>
       </c>
       <c r="B369">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C369" s="5">
-        <v>43703</v>
+        <v>43709</v>
       </c>
       <c r="D369" s="5">
         <v>43738</v>
@@ -6750,16 +6750,16 @@
     </row>
     <row r="370" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B370">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C370" s="5">
-        <v>43709</v>
+        <v>43739</v>
       </c>
       <c r="D370" s="5">
-        <v>43738</v>
+        <v>43914</v>
       </c>
       <c r="E370" t="s">
         <v>6</v>
@@ -6767,16 +6767,16 @@
     </row>
     <row r="371" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B371">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C371" s="5">
-        <v>43739</v>
+        <v>43770</v>
       </c>
       <c r="D371" s="5">
-        <v>43914</v>
+        <v>43951</v>
       </c>
       <c r="E371" t="s">
         <v>6</v>
@@ -6787,30 +6787,30 @@
         <v>7</v>
       </c>
       <c r="B372">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C372" s="5">
-        <v>43770</v>
+        <v>43831</v>
       </c>
       <c r="D372" s="5">
-        <v>43951</v>
+        <v>43914</v>
       </c>
       <c r="E372" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>7</v>
       </c>
       <c r="B373">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C373" s="5">
         <v>43831</v>
       </c>
       <c r="D373" s="5">
-        <v>43914</v>
+        <v>43951</v>
       </c>
       <c r="E373" t="s">
         <v>6</v>
@@ -6818,16 +6818,16 @@
     </row>
     <row r="374" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B374">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C374" s="5">
-        <v>43831</v>
+        <v>43862</v>
       </c>
       <c r="D374" s="5">
-        <v>43951</v>
+        <v>43914</v>
       </c>
       <c r="E374" t="s">
         <v>6</v>
@@ -6838,10 +6838,10 @@
         <v>5</v>
       </c>
       <c r="B375">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C375" s="5">
-        <v>43862</v>
+        <v>43891</v>
       </c>
       <c r="D375" s="5">
         <v>43914</v>
@@ -6855,7 +6855,7 @@
         <v>5</v>
       </c>
       <c r="B376">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C376" s="5">
         <v>43891</v>
@@ -6872,13 +6872,13 @@
         <v>5</v>
       </c>
       <c r="B377">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C377" s="5">
-        <v>43891</v>
+        <v>43958</v>
       </c>
       <c r="D377" s="5">
-        <v>43914</v>
+        <v>44104</v>
       </c>
       <c r="E377" t="s">
         <v>6</v>
@@ -6886,33 +6886,33 @@
     </row>
     <row r="378" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B378">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C378" s="5">
-        <v>43958</v>
+        <v>43983</v>
       </c>
       <c r="D378" s="5">
+        <v>44150</v>
+      </c>
+      <c r="E378" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="379" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A379" t="s">
+        <v>5</v>
+      </c>
+      <c r="B379">
+        <v>5</v>
+      </c>
+      <c r="C379" s="5">
+        <v>44013</v>
+      </c>
+      <c r="D379" s="5">
         <v>44104</v>
-      </c>
-      <c r="E378" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A379" t="s">
-        <v>7</v>
-      </c>
-      <c r="B379">
-        <v>10</v>
-      </c>
-      <c r="C379" s="5">
-        <v>43983</v>
-      </c>
-      <c r="D379" s="5">
-        <v>44150</v>
       </c>
       <c r="E379" t="s">
         <v>6</v>
@@ -6923,7 +6923,7 @@
         <v>5</v>
       </c>
       <c r="B380">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C380" s="5">
         <v>44013</v>
@@ -6935,12 +6935,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="381" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B381">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C381" s="5">
         <v>44013</v>
@@ -6957,13 +6957,13 @@
         <v>7</v>
       </c>
       <c r="B382">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C382" s="5">
         <v>44013</v>
       </c>
       <c r="D382" s="5">
-        <v>44104</v>
+        <v>44135</v>
       </c>
       <c r="E382" t="s">
         <v>6</v>
@@ -6974,7 +6974,7 @@
         <v>7</v>
       </c>
       <c r="B383">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C383" s="5">
         <v>44013</v>
@@ -6988,16 +6988,16 @@
     </row>
     <row r="384" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B384">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C384" s="5">
-        <v>44013</v>
+        <v>44028</v>
       </c>
       <c r="D384" s="5">
-        <v>44135</v>
+        <v>44104</v>
       </c>
       <c r="E384" t="s">
         <v>6</v>
@@ -7008,13 +7008,13 @@
         <v>5</v>
       </c>
       <c r="B385">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C385" s="5">
-        <v>44028</v>
+        <v>44105</v>
       </c>
       <c r="D385" s="5">
-        <v>44104</v>
+        <v>44316</v>
       </c>
       <c r="E385" t="s">
         <v>6</v>
@@ -7022,33 +7022,33 @@
     </row>
     <row r="386" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B386">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C386" s="5">
-        <v>44105</v>
+        <v>44197</v>
       </c>
       <c r="D386" s="5">
+        <v>44214</v>
+      </c>
+      <c r="E386" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="387" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A387" t="s">
+        <v>5</v>
+      </c>
+      <c r="B387">
+        <v>5</v>
+      </c>
+      <c r="C387" s="5">
+        <v>44256</v>
+      </c>
+      <c r="D387" s="5">
         <v>44316</v>
-      </c>
-      <c r="E386" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="387" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A387" t="s">
-        <v>7</v>
-      </c>
-      <c r="B387">
-        <v>10</v>
-      </c>
-      <c r="C387" s="5">
-        <v>44197</v>
-      </c>
-      <c r="D387" s="5">
-        <v>44214</v>
       </c>
       <c r="E387" t="s">
         <v>6</v>
@@ -7059,13 +7059,13 @@
         <v>5</v>
       </c>
       <c r="B388">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C388" s="5">
-        <v>44256</v>
+        <v>44317</v>
       </c>
       <c r="D388" s="5">
-        <v>44316</v>
+        <v>44469</v>
       </c>
       <c r="E388" t="s">
         <v>6</v>
@@ -7073,33 +7073,33 @@
     </row>
     <row r="389" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B389">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C389" s="5">
-        <v>44317</v>
+        <v>44363</v>
       </c>
       <c r="D389" s="5">
-        <v>44469</v>
+        <v>44500</v>
       </c>
       <c r="E389" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="390" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>7</v>
       </c>
       <c r="B390">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C390" s="5">
         <v>44363</v>
       </c>
       <c r="D390" s="5">
-        <v>44500</v>
+        <v>44469</v>
       </c>
       <c r="E390" t="s">
         <v>6</v>
@@ -7107,13 +7107,13 @@
     </row>
     <row r="391" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B391">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C391" s="5">
-        <v>44363</v>
+        <v>44378</v>
       </c>
       <c r="D391" s="5">
         <v>44469</v>
@@ -7127,7 +7127,7 @@
         <v>5</v>
       </c>
       <c r="B392">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C392" s="5">
         <v>44378</v>
@@ -7139,18 +7139,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="393" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>5</v>
       </c>
       <c r="B393">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C393" s="5">
         <v>44378</v>
       </c>
       <c r="D393" s="5">
-        <v>44469</v>
+        <v>44384</v>
       </c>
       <c r="E393" t="s">
         <v>6</v>
@@ -7158,16 +7158,16 @@
     </row>
     <row r="394" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B394">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C394" s="5">
         <v>44378</v>
       </c>
       <c r="D394" s="5">
-        <v>44384</v>
+        <v>44469</v>
       </c>
       <c r="E394" t="s">
         <v>6</v>
@@ -7175,13 +7175,13 @@
     </row>
     <row r="395" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B395">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C395" s="5">
-        <v>44378</v>
+        <v>44393</v>
       </c>
       <c r="D395" s="5">
         <v>44469</v>
@@ -7192,16 +7192,16 @@
     </row>
     <row r="396" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B396">
-        <v>9</v>
+        <v>81</v>
       </c>
       <c r="C396" s="5">
-        <v>44393</v>
+        <v>44409</v>
       </c>
       <c r="D396" s="5">
-        <v>44469</v>
+        <v>44458</v>
       </c>
       <c r="E396" t="s">
         <v>6</v>
@@ -7209,13 +7209,13 @@
     </row>
     <row r="397" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B397">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C397" s="5">
-        <v>44409</v>
+        <v>44422</v>
       </c>
       <c r="D397" s="5">
         <v>44458</v>
@@ -7226,19 +7226,16 @@
     </row>
     <row r="398" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B398">
-        <v>82</v>
+        <v>11</v>
       </c>
       <c r="C398" s="5">
-        <v>44422</v>
+        <v>44470</v>
       </c>
       <c r="D398" s="5">
-        <v>44458</v>
-      </c>
-      <c r="E398" t="s">
-        <v>6</v>
+        <v>44500</v>
       </c>
     </row>
     <row r="399" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -7246,47 +7243,50 @@
         <v>7</v>
       </c>
       <c r="B399">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C399" s="5">
         <v>44470</v>
       </c>
       <c r="D399" s="5">
-        <v>44500</v>
+        <v>44530</v>
       </c>
     </row>
     <row r="400" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B400">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C400" s="5">
         <v>44470</v>
       </c>
       <c r="D400" s="5">
-        <v>44530</v>
+        <v>44681</v>
+      </c>
+      <c r="E400" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="401" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B401">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C401" s="5">
-        <v>44470</v>
+        <v>44562</v>
       </c>
       <c r="D401" s="5">
-        <v>44681</v>
+        <v>44563</v>
       </c>
       <c r="E401" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="402" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>7</v>
       </c>
@@ -7294,16 +7294,16 @@
         <v>10</v>
       </c>
       <c r="C402" s="5">
-        <v>44562</v>
+        <v>44564</v>
       </c>
       <c r="D402" s="5">
-        <v>44563</v>
+        <v>44564</v>
       </c>
       <c r="E402" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="403" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>7</v>
       </c>
@@ -7311,16 +7311,16 @@
         <v>10</v>
       </c>
       <c r="C403" s="5">
-        <v>44564</v>
+        <v>44569</v>
       </c>
       <c r="D403" s="5">
-        <v>44564</v>
+        <v>44569</v>
       </c>
       <c r="E403" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="404" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>7</v>
       </c>
@@ -7328,16 +7328,16 @@
         <v>10</v>
       </c>
       <c r="C404" s="5">
-        <v>44569</v>
+        <v>44570</v>
       </c>
       <c r="D404" s="5">
-        <v>44569</v>
+        <v>44570</v>
       </c>
       <c r="E404" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="405" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>7</v>
       </c>
@@ -7345,16 +7345,16 @@
         <v>10</v>
       </c>
       <c r="C405" s="5">
-        <v>44570</v>
+        <v>44571</v>
       </c>
       <c r="D405" s="5">
-        <v>44570</v>
+        <v>44571</v>
       </c>
       <c r="E405" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="406" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>7</v>
       </c>
@@ -7362,16 +7362,16 @@
         <v>10</v>
       </c>
       <c r="C406" s="5">
-        <v>44571</v>
+        <v>44616</v>
       </c>
       <c r="D406" s="5">
-        <v>44571</v>
+        <v>44616</v>
       </c>
       <c r="E406" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="407" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>7</v>
       </c>
@@ -7379,16 +7379,16 @@
         <v>10</v>
       </c>
       <c r="C407" s="5">
-        <v>44616</v>
+        <v>44617</v>
       </c>
       <c r="D407" s="5">
-        <v>44616</v>
+        <v>44617</v>
       </c>
       <c r="E407" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="408" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>7</v>
       </c>
@@ -7396,16 +7396,16 @@
         <v>10</v>
       </c>
       <c r="C408" s="5">
-        <v>44617</v>
+        <v>44618</v>
       </c>
       <c r="D408" s="5">
-        <v>44617</v>
+        <v>44618</v>
       </c>
       <c r="E408" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="409" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>7</v>
       </c>
@@ -7413,16 +7413,16 @@
         <v>10</v>
       </c>
       <c r="C409" s="5">
-        <v>44618</v>
+        <v>44623</v>
       </c>
       <c r="D409" s="5">
-        <v>44618</v>
+        <v>44623</v>
       </c>
       <c r="E409" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="410" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>7</v>
       </c>
@@ -7430,16 +7430,16 @@
         <v>10</v>
       </c>
       <c r="C410" s="5">
-        <v>44623</v>
+        <v>44624</v>
       </c>
       <c r="D410" s="5">
-        <v>44623</v>
+        <v>44624</v>
       </c>
       <c r="E410" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="411" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>7</v>
       </c>
@@ -7447,16 +7447,16 @@
         <v>10</v>
       </c>
       <c r="C411" s="5">
-        <v>44624</v>
+        <v>44625</v>
       </c>
       <c r="D411" s="5">
-        <v>44624</v>
+        <v>44625</v>
       </c>
       <c r="E411" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="412" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>7</v>
       </c>
@@ -7464,16 +7464,16 @@
         <v>10</v>
       </c>
       <c r="C412" s="5">
-        <v>44625</v>
+        <v>44630</v>
       </c>
       <c r="D412" s="5">
-        <v>44625</v>
+        <v>44630</v>
       </c>
       <c r="E412" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="413" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>7</v>
       </c>
@@ -7481,16 +7481,16 @@
         <v>10</v>
       </c>
       <c r="C413" s="5">
-        <v>44630</v>
+        <v>44631</v>
       </c>
       <c r="D413" s="5">
-        <v>44630</v>
+        <v>44631</v>
       </c>
       <c r="E413" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="414" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>7</v>
       </c>
@@ -7498,16 +7498,16 @@
         <v>10</v>
       </c>
       <c r="C414" s="5">
-        <v>44631</v>
+        <v>44632</v>
       </c>
       <c r="D414" s="5">
-        <v>44631</v>
+        <v>44632</v>
       </c>
       <c r="E414" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="415" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>7</v>
       </c>
@@ -7515,16 +7515,16 @@
         <v>10</v>
       </c>
       <c r="C415" s="5">
-        <v>44632</v>
+        <v>44636</v>
       </c>
       <c r="D415" s="5">
-        <v>44632</v>
+        <v>44637</v>
       </c>
       <c r="E415" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="416" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>7</v>
       </c>
@@ -7532,16 +7532,16 @@
         <v>10</v>
       </c>
       <c r="C416" s="5">
-        <v>44636</v>
+        <v>44638</v>
       </c>
       <c r="D416" s="5">
-        <v>44637</v>
+        <v>44638</v>
       </c>
       <c r="E416" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="417" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>7</v>
       </c>
@@ -7549,16 +7549,16 @@
         <v>10</v>
       </c>
       <c r="C417" s="5">
-        <v>44638</v>
+        <v>44639</v>
       </c>
       <c r="D417" s="5">
-        <v>44638</v>
+        <v>44639</v>
       </c>
       <c r="E417" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="418" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>7</v>
       </c>
@@ -7566,16 +7566,16 @@
         <v>10</v>
       </c>
       <c r="C418" s="5">
-        <v>44639</v>
+        <v>44640</v>
       </c>
       <c r="D418" s="5">
-        <v>44639</v>
+        <v>44640</v>
       </c>
       <c r="E418" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="419" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
         <v>7</v>
       </c>
@@ -7583,16 +7583,16 @@
         <v>10</v>
       </c>
       <c r="C419" s="5">
-        <v>44640</v>
+        <v>44641</v>
       </c>
       <c r="D419" s="5">
-        <v>44640</v>
+        <v>44644</v>
       </c>
       <c r="E419" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="420" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>7</v>
       </c>
@@ -7600,16 +7600,16 @@
         <v>10</v>
       </c>
       <c r="C420" s="5">
-        <v>44641</v>
+        <v>44645</v>
       </c>
       <c r="D420" s="5">
-        <v>44644</v>
+        <v>44645</v>
       </c>
       <c r="E420" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="421" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>7</v>
       </c>
@@ -7617,16 +7617,16 @@
         <v>10</v>
       </c>
       <c r="C421" s="5">
-        <v>44645</v>
+        <v>44646</v>
       </c>
       <c r="D421" s="5">
-        <v>44645</v>
+        <v>44646</v>
       </c>
       <c r="E421" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="422" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>7</v>
       </c>
@@ -7634,16 +7634,16 @@
         <v>10</v>
       </c>
       <c r="C422" s="5">
-        <v>44646</v>
+        <v>44647</v>
       </c>
       <c r="D422" s="5">
-        <v>44646</v>
+        <v>44647</v>
       </c>
       <c r="E422" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="423" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>7</v>
       </c>
@@ -7651,27 +7651,27 @@
         <v>10</v>
       </c>
       <c r="C423" s="5">
-        <v>44647</v>
+        <v>44648</v>
       </c>
       <c r="D423" s="5">
-        <v>44647</v>
+        <v>44651</v>
       </c>
       <c r="E423" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="424" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B424">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C424" s="5">
-        <v>44648</v>
+        <v>44700</v>
       </c>
       <c r="D424" s="5">
-        <v>44651</v>
+        <v>44798</v>
       </c>
       <c r="E424" t="s">
         <v>6</v>
@@ -7679,19 +7679,16 @@
     </row>
     <row r="425" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B425">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C425" s="5">
-        <v>44700</v>
+        <v>44713</v>
       </c>
       <c r="D425" s="5">
-        <v>44798</v>
-      </c>
-      <c r="E425" t="s">
-        <v>6</v>
+        <v>44714</v>
       </c>
     </row>
     <row r="426" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -7702,10 +7699,10 @@
         <v>11</v>
       </c>
       <c r="C426" s="5">
-        <v>44713</v>
+        <v>44715</v>
       </c>
       <c r="D426" s="5">
-        <v>44714</v>
+        <v>44715</v>
       </c>
     </row>
     <row r="427" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -7713,27 +7710,30 @@
         <v>7</v>
       </c>
       <c r="B427">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C427" s="5">
-        <v>44715</v>
+        <v>44728</v>
       </c>
       <c r="D427" s="5">
-        <v>44715</v>
-      </c>
-    </row>
-    <row r="428" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44865</v>
+      </c>
+      <c r="E427" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="428" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B428">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C428" s="5">
-        <v>44728</v>
+        <v>44743</v>
       </c>
       <c r="D428" s="5">
-        <v>44865</v>
+        <v>44746</v>
       </c>
       <c r="E428" t="s">
         <v>6</v>
@@ -7744,13 +7744,13 @@
         <v>5</v>
       </c>
       <c r="B429">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C429" s="5">
         <v>44743</v>
       </c>
       <c r="D429" s="5">
-        <v>44746</v>
+        <v>44765</v>
       </c>
       <c r="E429" t="s">
         <v>6</v>
@@ -7758,19 +7758,16 @@
     </row>
     <row r="430" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B430">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C430" s="5">
         <v>44743</v>
       </c>
       <c r="D430" s="5">
-        <v>44765</v>
-      </c>
-      <c r="E430" t="s">
-        <v>6</v>
+        <v>44743</v>
       </c>
     </row>
     <row r="431" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -7778,13 +7775,13 @@
         <v>7</v>
       </c>
       <c r="B431">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C431" s="5">
         <v>44743</v>
       </c>
       <c r="D431" s="5">
-        <v>44743</v>
+        <v>44834</v>
       </c>
     </row>
     <row r="432" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -7792,76 +7789,76 @@
         <v>7</v>
       </c>
       <c r="B432">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C432" s="5">
-        <v>44743</v>
+        <v>44744</v>
       </c>
       <c r="D432" s="5">
-        <v>44834</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="433" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B433">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C433" s="5">
-        <v>44744</v>
+        <v>44748</v>
       </c>
       <c r="D433" s="5">
-        <v>44744</v>
+        <v>44748</v>
+      </c>
+      <c r="E433" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="434" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B434">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C434" s="5">
         <v>44748</v>
       </c>
       <c r="D434" s="5">
-        <v>44748</v>
-      </c>
-      <c r="E434" t="s">
-        <v>6</v>
+        <v>44749</v>
       </c>
     </row>
     <row r="435" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B435">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C435" s="5">
-        <v>44748</v>
+        <v>44750</v>
       </c>
       <c r="D435" s="5">
-        <v>44749</v>
+        <f>C435</f>
+        <v>44750</v>
+      </c>
+      <c r="E435" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="436" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B436">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C436" s="5">
         <v>44750</v>
       </c>
       <c r="D436" s="5">
-        <f>C436</f>
         <v>44750</v>
-      </c>
-      <c r="E436" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="437" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -7872,24 +7869,28 @@
         <v>11</v>
       </c>
       <c r="C437" s="5">
-        <v>44750</v>
+        <v>44751</v>
       </c>
       <c r="D437" s="5">
-        <v>44750</v>
+        <v>44751</v>
       </c>
     </row>
     <row r="438" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B438">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C438" s="5">
-        <v>44751</v>
+        <v>44752</v>
       </c>
       <c r="D438" s="5">
-        <v>44751</v>
+        <f>C438</f>
+        <v>44752</v>
+      </c>
+      <c r="E438" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="439" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -7900,11 +7901,11 @@
         <v>5</v>
       </c>
       <c r="C439" s="5">
-        <v>44752</v>
+        <v>44754</v>
       </c>
       <c r="D439" s="5">
         <f>C439</f>
-        <v>44752</v>
+        <v>44754</v>
       </c>
       <c r="E439" t="s">
         <v>6</v>
@@ -7918,29 +7919,28 @@
         <v>5</v>
       </c>
       <c r="C440" s="5">
-        <v>44754</v>
+        <v>44756</v>
       </c>
       <c r="D440" s="5">
         <f>C440</f>
-        <v>44754</v>
+        <v>44756</v>
       </c>
       <c r="E440" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="441" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
         <v>5</v>
       </c>
       <c r="B441">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C441" s="5">
         <v>44756</v>
       </c>
       <c r="D441" s="5">
-        <f>C441</f>
-        <v>44756</v>
+        <v>44758</v>
       </c>
       <c r="E441" t="s">
         <v>6</v>
@@ -7951,7 +7951,7 @@
         <v>5</v>
       </c>
       <c r="B442">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C442" s="5">
         <v>44756</v>
@@ -7968,12 +7968,13 @@
         <v>5</v>
       </c>
       <c r="B443">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C443" s="5">
-        <v>44756</v>
+        <v>44758</v>
       </c>
       <c r="D443" s="5">
+        <f>C443</f>
         <v>44758</v>
       </c>
       <c r="E443" t="s">
@@ -7988,11 +7989,11 @@
         <v>5</v>
       </c>
       <c r="C444" s="5">
-        <v>44758</v>
+        <v>44760</v>
       </c>
       <c r="D444" s="5">
         <f>C444</f>
-        <v>44758</v>
+        <v>44760</v>
       </c>
       <c r="E444" t="s">
         <v>6</v>
@@ -8006,29 +8007,28 @@
         <v>5</v>
       </c>
       <c r="C445" s="5">
-        <v>44760</v>
+        <v>44762</v>
       </c>
       <c r="D445" s="5">
         <f>C445</f>
-        <v>44760</v>
+        <v>44762</v>
       </c>
       <c r="E445" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="446" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
         <v>5</v>
       </c>
       <c r="B446">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C446" s="5">
-        <v>44762</v>
+        <v>44763</v>
       </c>
       <c r="D446" s="5">
-        <f>C446</f>
-        <v>44762</v>
+        <v>44765</v>
       </c>
       <c r="E446" t="s">
         <v>6</v>
@@ -8039,7 +8039,7 @@
         <v>5</v>
       </c>
       <c r="B447">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C447" s="5">
         <v>44763</v>
@@ -8056,13 +8056,14 @@
         <v>5</v>
       </c>
       <c r="B448">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C448" s="5">
-        <v>44763</v>
+        <v>44764</v>
       </c>
       <c r="D448" s="5">
-        <v>44765</v>
+        <f>C448</f>
+        <v>44764</v>
       </c>
       <c r="E448" t="s">
         <v>6</v>
@@ -8076,11 +8077,10 @@
         <v>5</v>
       </c>
       <c r="C449" s="5">
-        <v>44764</v>
+        <v>44766</v>
       </c>
       <c r="D449" s="5">
-        <f>C449</f>
-        <v>44764</v>
+        <v>44832</v>
       </c>
       <c r="E449" t="s">
         <v>6</v>
@@ -8091,10 +8091,10 @@
         <v>5</v>
       </c>
       <c r="B450">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C450" s="5">
-        <v>44766</v>
+        <v>44769</v>
       </c>
       <c r="D450" s="5">
         <v>44832</v>
@@ -8103,18 +8103,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="451" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
         <v>5</v>
       </c>
       <c r="B451">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C451" s="5">
-        <v>44769</v>
+        <v>44770</v>
       </c>
       <c r="D451" s="5">
-        <v>44832</v>
+        <v>44772</v>
       </c>
       <c r="E451" t="s">
         <v>6</v>
@@ -8125,13 +8125,13 @@
         <v>5</v>
       </c>
       <c r="B452">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C452" s="5">
         <v>44770</v>
       </c>
       <c r="D452" s="5">
-        <v>44772</v>
+        <v>44829</v>
       </c>
       <c r="E452" t="s">
         <v>6</v>
@@ -8139,19 +8139,16 @@
     </row>
     <row r="453" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B453">
-        <v>9</v>
+        <v>81</v>
       </c>
       <c r="C453" s="5">
-        <v>44770</v>
+        <v>44774</v>
       </c>
       <c r="D453" s="5">
-        <v>44829</v>
-      </c>
-      <c r="E453" t="s">
-        <v>6</v>
+        <v>44834</v>
       </c>
     </row>
     <row r="454" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8159,13 +8156,13 @@
         <v>7</v>
       </c>
       <c r="B454">
-        <v>81</v>
+        <v>11</v>
       </c>
       <c r="C454" s="5">
-        <v>44774</v>
+        <v>44776</v>
       </c>
       <c r="D454" s="5">
-        <v>44834</v>
+        <v>44777</v>
       </c>
     </row>
     <row r="455" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8176,10 +8173,10 @@
         <v>11</v>
       </c>
       <c r="C455" s="5">
-        <v>44776</v>
+        <v>44778</v>
       </c>
       <c r="D455" s="5">
-        <v>44777</v>
+        <v>44778</v>
       </c>
     </row>
     <row r="456" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8190,10 +8187,10 @@
         <v>11</v>
       </c>
       <c r="C456" s="5">
-        <v>44778</v>
+        <v>44779</v>
       </c>
       <c r="D456" s="5">
-        <v>44778</v>
+        <v>44779</v>
       </c>
     </row>
     <row r="457" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8204,10 +8201,10 @@
         <v>11</v>
       </c>
       <c r="C457" s="5">
-        <v>44779</v>
+        <v>44783</v>
       </c>
       <c r="D457" s="5">
-        <v>44779</v>
+        <v>44784</v>
       </c>
     </row>
     <row r="458" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8218,10 +8215,10 @@
         <v>11</v>
       </c>
       <c r="C458" s="5">
-        <v>44783</v>
+        <v>44785</v>
       </c>
       <c r="D458" s="5">
-        <v>44784</v>
+        <v>44785</v>
       </c>
     </row>
     <row r="459" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8232,55 +8229,55 @@
         <v>11</v>
       </c>
       <c r="C459" s="5">
-        <v>44785</v>
+        <v>44786</v>
       </c>
       <c r="D459" s="5">
-        <v>44785</v>
+        <v>44786</v>
       </c>
     </row>
     <row r="460" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B460">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="C460" s="5">
         <v>44786</v>
       </c>
       <c r="D460" s="5">
-        <v>44786</v>
-      </c>
-    </row>
-    <row r="461" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>44823</v>
+      </c>
+    </row>
+    <row r="461" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
         <v>5</v>
       </c>
       <c r="B461">
-        <v>82</v>
+        <v>7</v>
       </c>
       <c r="C461" s="5">
-        <v>44786</v>
+        <v>44789</v>
       </c>
       <c r="D461" s="5">
-        <v>44823</v>
+        <v>44834</v>
+      </c>
+      <c r="E461" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="462" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B462">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C462" s="5">
-        <v>44789</v>
+        <v>44790</v>
       </c>
       <c r="D462" s="5">
-        <v>44834</v>
-      </c>
-      <c r="E462" t="s">
-        <v>6</v>
+        <v>44791</v>
       </c>
     </row>
     <row r="463" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8291,10 +8288,10 @@
         <v>11</v>
       </c>
       <c r="C463" s="5">
-        <v>44790</v>
+        <v>44792</v>
       </c>
       <c r="D463" s="5">
-        <v>44791</v>
+        <v>44792</v>
       </c>
     </row>
     <row r="464" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8305,10 +8302,10 @@
         <v>11</v>
       </c>
       <c r="C464" s="5">
-        <v>44792</v>
+        <v>44793</v>
       </c>
       <c r="D464" s="5">
-        <v>44792</v>
+        <v>44793</v>
       </c>
     </row>
     <row r="465" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8319,10 +8316,10 @@
         <v>11</v>
       </c>
       <c r="C465" s="5">
-        <v>44793</v>
+        <v>44794</v>
       </c>
       <c r="D465" s="5">
-        <v>44793</v>
+        <v>44794</v>
       </c>
     </row>
     <row r="466" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8333,10 +8330,10 @@
         <v>11</v>
       </c>
       <c r="C466" s="5">
-        <v>44794</v>
+        <v>44795</v>
       </c>
       <c r="D466" s="5">
-        <v>44794</v>
+        <v>44798</v>
       </c>
     </row>
     <row r="467" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8347,10 +8344,10 @@
         <v>11</v>
       </c>
       <c r="C467" s="5">
-        <v>44795</v>
+        <v>44799</v>
       </c>
       <c r="D467" s="5">
-        <v>44798</v>
+        <v>44799</v>
       </c>
     </row>
     <row r="468" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8361,10 +8358,10 @@
         <v>11</v>
       </c>
       <c r="C468" s="5">
-        <v>44799</v>
+        <v>44800</v>
       </c>
       <c r="D468" s="5">
-        <v>44799</v>
+        <v>44800</v>
       </c>
     </row>
     <row r="469" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8375,10 +8372,10 @@
         <v>11</v>
       </c>
       <c r="C469" s="5">
-        <v>44800</v>
+        <v>44801</v>
       </c>
       <c r="D469" s="5">
-        <v>44800</v>
+        <v>44801</v>
       </c>
     </row>
     <row r="470" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8389,41 +8386,41 @@
         <v>11</v>
       </c>
       <c r="C470" s="5">
-        <v>44801</v>
+        <v>44802</v>
       </c>
       <c r="D470" s="5">
-        <v>44801</v>
+        <v>44805</v>
       </c>
     </row>
     <row r="471" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B471">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C471" s="5">
-        <v>44802</v>
+        <v>44804</v>
       </c>
       <c r="D471" s="5">
-        <v>44805</v>
+        <v>44834</v>
+      </c>
+      <c r="E471" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="472" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B472">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C472" s="5">
-        <v>44804</v>
+        <v>44806</v>
       </c>
       <c r="D472" s="5">
-        <v>44834</v>
-      </c>
-      <c r="E472" t="s">
-        <v>6</v>
+        <v>44806</v>
       </c>
     </row>
     <row r="473" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8434,10 +8431,10 @@
         <v>11</v>
       </c>
       <c r="C473" s="5">
-        <v>44806</v>
+        <v>44807</v>
       </c>
       <c r="D473" s="5">
-        <v>44806</v>
+        <v>44807</v>
       </c>
     </row>
     <row r="474" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8448,10 +8445,10 @@
         <v>11</v>
       </c>
       <c r="C474" s="5">
-        <v>44807</v>
+        <v>44808</v>
       </c>
       <c r="D474" s="5">
-        <v>44807</v>
+        <v>44809</v>
       </c>
     </row>
     <row r="475" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8462,10 +8459,10 @@
         <v>11</v>
       </c>
       <c r="C475" s="5">
-        <v>44808</v>
+        <v>44810</v>
       </c>
       <c r="D475" s="5">
-        <v>44809</v>
+        <v>44812</v>
       </c>
     </row>
     <row r="476" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8476,10 +8473,10 @@
         <v>11</v>
       </c>
       <c r="C476" s="5">
-        <v>44810</v>
+        <v>44813</v>
       </c>
       <c r="D476" s="5">
-        <v>44812</v>
+        <v>44813</v>
       </c>
     </row>
     <row r="477" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8490,10 +8487,10 @@
         <v>11</v>
       </c>
       <c r="C477" s="5">
-        <v>44813</v>
+        <v>44814</v>
       </c>
       <c r="D477" s="5">
-        <v>44813</v>
+        <v>44814</v>
       </c>
     </row>
     <row r="478" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8504,10 +8501,10 @@
         <v>11</v>
       </c>
       <c r="C478" s="5">
-        <v>44814</v>
+        <v>44815</v>
       </c>
       <c r="D478" s="5">
-        <v>44814</v>
+        <v>44815</v>
       </c>
     </row>
     <row r="479" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8518,10 +8515,10 @@
         <v>11</v>
       </c>
       <c r="C479" s="5">
-        <v>44815</v>
+        <v>44816</v>
       </c>
       <c r="D479" s="5">
-        <v>44815</v>
+        <v>44819</v>
       </c>
     </row>
     <row r="480" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8532,10 +8529,10 @@
         <v>11</v>
       </c>
       <c r="C480" s="5">
-        <v>44816</v>
+        <v>44820</v>
       </c>
       <c r="D480" s="5">
-        <v>44819</v>
+        <v>44820</v>
       </c>
     </row>
     <row r="481" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8546,10 +8543,10 @@
         <v>11</v>
       </c>
       <c r="C481" s="5">
-        <v>44820</v>
+        <v>44821</v>
       </c>
       <c r="D481" s="5">
-        <v>44820</v>
+        <v>44821</v>
       </c>
     </row>
     <row r="482" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8560,10 +8557,10 @@
         <v>11</v>
       </c>
       <c r="C482" s="5">
-        <v>44821</v>
+        <v>44822</v>
       </c>
       <c r="D482" s="5">
-        <v>44821</v>
+        <v>44822</v>
       </c>
     </row>
     <row r="483" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8574,10 +8571,10 @@
         <v>11</v>
       </c>
       <c r="C483" s="5">
-        <v>44822</v>
+        <v>44823</v>
       </c>
       <c r="D483" s="5">
-        <v>44822</v>
+        <v>44826</v>
       </c>
     </row>
     <row r="484" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8588,10 +8585,10 @@
         <v>11</v>
       </c>
       <c r="C484" s="5">
-        <v>44823</v>
+        <v>44827</v>
       </c>
       <c r="D484" s="5">
-        <v>44826</v>
+        <v>44827</v>
       </c>
     </row>
     <row r="485" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8602,10 +8599,10 @@
         <v>11</v>
       </c>
       <c r="C485" s="5">
-        <v>44827</v>
+        <v>44828</v>
       </c>
       <c r="D485" s="5">
-        <v>44827</v>
+        <v>44828</v>
       </c>
     </row>
     <row r="486" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8616,10 +8613,10 @@
         <v>11</v>
       </c>
       <c r="C486" s="5">
-        <v>44828</v>
+        <v>44829</v>
       </c>
       <c r="D486" s="5">
-        <v>44828</v>
+        <v>44829</v>
       </c>
     </row>
     <row r="487" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8630,10 +8627,10 @@
         <v>11</v>
       </c>
       <c r="C487" s="5">
-        <v>44829</v>
+        <v>44830</v>
       </c>
       <c r="D487" s="5">
-        <v>44829</v>
+        <v>44833</v>
       </c>
     </row>
     <row r="488" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8644,10 +8641,10 @@
         <v>11</v>
       </c>
       <c r="C488" s="5">
-        <v>44830</v>
+        <v>44834</v>
       </c>
       <c r="D488" s="5">
-        <v>44833</v>
+        <v>44834</v>
       </c>
     </row>
     <row r="489" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8658,10 +8655,10 @@
         <v>11</v>
       </c>
       <c r="C489" s="5">
-        <v>44834</v>
+        <v>44835</v>
       </c>
       <c r="D489" s="5">
-        <v>44834</v>
+        <v>44865</v>
       </c>
     </row>
     <row r="490" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -8669,7 +8666,7 @@
         <v>7</v>
       </c>
       <c r="B490">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C490" s="5">
         <v>44835</v>
@@ -8680,62 +8677,48 @@
     </row>
     <row r="491" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B491">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C491" s="5">
         <v>44835</v>
       </c>
       <c r="D491" s="5">
-        <v>44865</v>
+        <v>45046</v>
+      </c>
+      <c r="E491" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="492" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B492">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="C492" s="5">
         <v>44835</v>
       </c>
       <c r="D492" s="5">
-        <v>45046</v>
-      </c>
-      <c r="E492" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="493" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A493" t="s">
-        <v>7</v>
-      </c>
-      <c r="B493">
-        <v>81</v>
-      </c>
-      <c r="C493" s="5">
-        <v>44835</v>
-      </c>
-      <c r="D493" s="5">
         <v>44843</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E493" xr:uid="{9536AF9F-EFE7-469A-8B3B-7525E4B6BE61}">
+  <autoFilter ref="A1:E492" xr:uid="{9536AF9F-EFE7-469A-8B3B-7525E4B6BE61}">
     <filterColumn colId="1">
       <filters>
-        <filter val="10"/>
+        <filter val="7"/>
       </filters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:E450">
-      <sortCondition ref="C264:C493"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:E449">
+      <sortCondition ref="C264:C492"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E493">
-    <sortCondition ref="C207:C493"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E492">
+    <sortCondition ref="C207:C492"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8744,6 +8727,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -8754,15 +8746,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9006,6 +8989,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{902BFF43-0B71-4183-AE7E-FA994EED3F0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37A00794-6F8A-440F-8D17-1F18CC3F357B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9013,14 +9004,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="671c5c8a-d1dd-40a7-bcfd-3ed591bedb5d"/>
     <ds:schemaRef ds:uri="62120a19-a38a-4c78-8e86-03b65bdcf4fa"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{902BFF43-0B71-4183-AE7E-FA994EED3F0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>